<commit_message>
Alteração dos calculos dos card - Callipers com by pass e vedações originais
</commit_message>
<xml_diff>
--- a/Analise-de-substituicao-de-calliper.xlsx
+++ b/Analise-de-substituicao-de-calliper.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://voltaliagroup-my.sharepoint.com/personal/de_ferreira_voltalia_com/Documents/09 - Arquivos WEG/dashboard-Calliper-Eolico/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de.ferreira\Desktop\dashboard-substituicao-calliper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{657E3F6A-534B-4085-AC4F-C1CB1243E543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07E28C66-21C9-4720-8101-E385DF57644B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAA4B9E-2949-4689-B828-639CA0A4177C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FA9E4268-8FE5-4DC5-93B3-4B3954182B74}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FA9E4268-8FE5-4DC5-93B3-4B3954182B74}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="87">
   <si>
     <t>-</t>
   </si>
@@ -245,9 +246,6 @@
     <t>SI-43</t>
   </si>
   <si>
-    <t>Substituído parcialmente</t>
-  </si>
-  <si>
     <t>SI-41</t>
   </si>
   <si>
@@ -294,6 +292,12 @@
   </si>
   <si>
     <t>CONDICAO CALLIPER</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>No codigo</t>
   </si>
 </sst>
 </file>
@@ -303,7 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,13 +322,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -381,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,6 +432,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,10 +1045,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B081B7-EA77-45F0-9C85-62DDCE899F30}">
-  <dimension ref="A1:N236"/>
+  <dimension ref="A1:M236"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,38 +1062,40 @@
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="E1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>61</v>
       </c>
@@ -1073,7 +1103,7 @@
         <v>45798</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
@@ -1088,13 +1118,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>61</v>
       </c>
@@ -1102,7 +1132,7 @@
         <v>45820</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -1117,13 +1147,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>61</v>
       </c>
@@ -1131,7 +1161,7 @@
         <v>45888</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -1146,13 +1176,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>61</v>
       </c>
@@ -1160,7 +1190,7 @@
         <v>45888</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -1175,13 +1205,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -1189,7 +1219,7 @@
         <v>45820</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>2</v>
@@ -1204,13 +1234,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
@@ -1218,7 +1248,7 @@
         <v>45667</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -1233,13 +1263,13 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>61</v>
       </c>
@@ -1247,7 +1277,7 @@
         <v>45622</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>7</v>
@@ -1262,13 +1292,13 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>61</v>
       </c>
@@ -1276,7 +1306,7 @@
         <v>45761</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -1291,13 +1321,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
@@ -1305,7 +1335,7 @@
         <v>45761</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>5</v>
@@ -1320,13 +1350,13 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
@@ -1334,7 +1364,7 @@
         <v>45868</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
@@ -1349,14 +1379,14 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N11" s="11"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>61</v>
       </c>
@@ -1364,7 +1394,7 @@
         <v>45855</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -1379,13 +1409,13 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
@@ -1393,7 +1423,7 @@
         <v>45901</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
@@ -1408,19 +1438,21 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -1441,13 +1473,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>5</v>
@@ -1468,7 +1502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
@@ -1476,7 +1510,7 @@
         <v>45901</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>2</v>
@@ -1491,7 +1525,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>10</v>
@@ -1505,7 +1539,7 @@
         <v>45809</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -1520,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>0</v>
@@ -1534,7 +1568,7 @@
         <v>45832</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
@@ -1549,7 +1583,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>0</v>
@@ -1563,7 +1597,7 @@
         <v>45621</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -1578,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>0</v>
@@ -1592,7 +1626,7 @@
         <v>45832</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>5</v>
@@ -1607,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>0</v>
@@ -1621,7 +1655,7 @@
         <v>45809</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>2</v>
@@ -1636,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>0</v>
@@ -1650,7 +1684,7 @@
         <v>45649</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -1665,7 +1699,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>0</v>
@@ -1679,7 +1713,7 @@
         <v>45712</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>7</v>
@@ -1694,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>0</v>
@@ -1708,7 +1742,7 @@
         <v>45709</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
@@ -1723,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>0</v>
@@ -1737,7 +1771,7 @@
         <v>45709</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>5</v>
@@ -1752,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>0</v>
@@ -1766,7 +1800,7 @@
         <v>45712</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>2</v>
@@ -1781,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>0</v>
@@ -1795,7 +1829,7 @@
         <v>45689</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>8</v>
@@ -1810,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>0</v>
@@ -1824,7 +1858,7 @@
         <v>45447</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>7</v>
@@ -1839,7 +1873,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>0</v>
@@ -1853,7 +1887,7 @@
         <v>45689</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -1868,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>0</v>
@@ -1882,7 +1916,7 @@
         <v>45824</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
@@ -1894,10 +1928,10 @@
         <v>45824</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>0</v>
@@ -1911,7 +1945,7 @@
         <v>45824</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>2</v>
@@ -1923,10 +1957,10 @@
         <v>45824</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>0</v>
@@ -1955,7 +1989,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>0</v>
@@ -1984,7 +2018,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>10</v>
@@ -2013,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>0</v>
@@ -2042,7 +2076,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>10</v>
@@ -2071,7 +2105,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>10</v>
@@ -2082,7 +2116,7 @@
         <v>61</v>
       </c>
       <c r="B37" s="1">
-        <v>45855</v>
+        <v>45930</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>67</v>
@@ -2100,7 +2134,7 @@
         <v>1</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>10</v>
@@ -2111,7 +2145,7 @@
         <v>61</v>
       </c>
       <c r="B38" s="1">
-        <v>45855</v>
+        <v>45929</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>67</v>
@@ -2129,7 +2163,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>10</v>
@@ -2140,7 +2174,7 @@
         <v>61</v>
       </c>
       <c r="B39" s="1">
-        <v>45855</v>
+        <v>45930</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>67</v>
@@ -2158,7 +2192,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>10</v>
@@ -2169,7 +2203,7 @@
         <v>61</v>
       </c>
       <c r="B40" s="1">
-        <v>45855</v>
+        <v>45930</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>67</v>
@@ -2187,7 +2221,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>10</v>
@@ -2198,7 +2232,7 @@
         <v>61</v>
       </c>
       <c r="B41" s="1">
-        <v>45855</v>
+        <v>45929</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>67</v>
@@ -2216,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>10</v>
@@ -2245,7 +2279,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>63</v>
@@ -2274,7 +2308,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>66</v>
@@ -2303,7 +2337,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>65</v>
@@ -2332,7 +2366,7 @@
         <v>1</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>37</v>
@@ -2361,7 +2395,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>63</v>
@@ -2390,7 +2424,7 @@
         <v>1</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>0</v>
@@ -2419,7 +2453,7 @@
         <v>1</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>0</v>
@@ -2448,7 +2482,7 @@
         <v>1</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>0</v>
@@ -2477,7 +2511,7 @@
         <v>1</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>0</v>
@@ -2506,7 +2540,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>0</v>
@@ -2535,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>0</v>
@@ -2564,7 +2598,7 @@
         <v>1</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>0</v>
@@ -2575,7 +2609,7 @@
         <v>61</v>
       </c>
       <c r="B54" s="1">
-        <v>45862</v>
+        <v>45936</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>60</v>
@@ -2593,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>10</v>
@@ -2604,7 +2638,7 @@
         <v>61</v>
       </c>
       <c r="B55" s="1">
-        <v>45862</v>
+        <v>45936</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>60</v>
@@ -2622,7 +2656,7 @@
         <v>1</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>10</v>
@@ -2633,7 +2667,7 @@
         <v>61</v>
       </c>
       <c r="B56" s="1">
-        <v>45862</v>
+        <v>45936</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>60</v>
@@ -2651,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>10</v>
@@ -2661,7 +2695,9 @@
       <c r="A57" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B57" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C57" s="2" t="s">
         <v>59</v>
       </c>
@@ -2707,7 +2743,7 @@
         <v>1</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>0</v>
@@ -2736,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>0</v>
@@ -2765,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>0</v>
@@ -2794,7 +2830,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>0</v>
@@ -2823,7 +2859,7 @@
         <v>1</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>0</v>
@@ -2852,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>0</v>
@@ -2881,7 +2917,7 @@
         <v>1</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>0</v>
@@ -2910,7 +2946,7 @@
         <v>1</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>0</v>
@@ -2939,7 +2975,7 @@
         <v>1</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>0</v>
@@ -2968,7 +3004,7 @@
         <v>1</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>0</v>
@@ -2997,7 +3033,7 @@
         <v>1</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>0</v>
@@ -3026,7 +3062,7 @@
         <v>1</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>0</v>
@@ -3055,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>0</v>
@@ -3084,7 +3120,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>0</v>
@@ -3113,7 +3149,7 @@
         <v>1</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>0</v>
@@ -3142,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>0</v>
@@ -3171,7 +3207,7 @@
         <v>1</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>0</v>
@@ -3200,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>0</v>
@@ -3229,7 +3265,7 @@
         <v>1</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>0</v>
@@ -3258,7 +3294,7 @@
         <v>1</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>0</v>
@@ -3287,7 +3323,7 @@
         <v>1</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>0</v>
@@ -3297,7 +3333,9 @@
       <c r="A79" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B79" s="1"/>
+      <c r="B79" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="C79" s="2" t="s">
         <v>55</v>
       </c>
@@ -3324,7 +3362,9 @@
       <c r="A80" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B80" s="1"/>
+      <c r="B80" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="C80" s="2" t="s">
         <v>55</v>
       </c>
@@ -3351,7 +3391,9 @@
       <c r="A81" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B81" s="1"/>
+      <c r="B81" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="C81" s="2" t="s">
         <v>55</v>
       </c>
@@ -3397,7 +3439,7 @@
         <v>1</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>10</v>
@@ -3426,7 +3468,7 @@
         <v>1</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>10</v>
@@ -3455,7 +3497,7 @@
         <v>1</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>10</v>
@@ -3484,7 +3526,7 @@
         <v>1</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>10</v>
@@ -3513,7 +3555,7 @@
         <v>1</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>10</v>
@@ -3542,7 +3584,7 @@
         <v>1</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>0</v>
@@ -3571,7 +3613,7 @@
         <v>1</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>0</v>
@@ -3600,7 +3642,7 @@
         <v>1</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>0</v>
@@ -3629,7 +3671,7 @@
         <v>1</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>0</v>
@@ -3658,7 +3700,7 @@
         <v>1</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>0</v>
@@ -3687,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>0</v>
@@ -3716,7 +3758,7 @@
         <v>1</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>0</v>
@@ -3745,7 +3787,7 @@
         <v>1</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>0</v>
@@ -3774,7 +3816,7 @@
         <v>1</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>0</v>
@@ -3803,7 +3845,7 @@
         <v>1</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>0</v>
@@ -3832,7 +3874,7 @@
         <v>1</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>0</v>
@@ -3861,7 +3903,7 @@
         <v>1</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>0</v>
@@ -3890,7 +3932,7 @@
         <v>1</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>0</v>
@@ -3919,7 +3961,7 @@
         <v>1</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>0</v>
@@ -3948,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>0</v>
@@ -3977,7 +4019,7 @@
         <v>1</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>10</v>
@@ -4006,7 +4048,7 @@
         <v>1</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>10</v>
@@ -4035,7 +4077,7 @@
         <v>1</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>10</v>
@@ -4064,7 +4106,7 @@
         <v>1</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>10</v>
@@ -4093,7 +4135,7 @@
         <v>1</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>10</v>
@@ -4118,11 +4160,11 @@
       <c r="F107" s="3">
         <v>45835</v>
       </c>
-      <c r="G107" s="2" t="s">
+      <c r="G107" s="12" t="s">
         <v>1</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>0</v>
@@ -4151,7 +4193,7 @@
         <v>1</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>0</v>
@@ -4180,7 +4222,7 @@
         <v>1</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>0</v>
@@ -4209,7 +4251,7 @@
         <v>1</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>0</v>
@@ -4238,7 +4280,7 @@
         <v>1</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>0</v>
@@ -4267,7 +4309,7 @@
         <v>1</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>37</v>
@@ -4296,7 +4338,7 @@
         <v>1</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>47</v>
@@ -4325,7 +4367,7 @@
         <v>1</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>10</v>
@@ -4354,7 +4396,7 @@
         <v>1</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>10</v>
@@ -4383,7 +4425,7 @@
         <v>1</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>10</v>
@@ -4412,7 +4454,7 @@
         <v>1</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>10</v>
@@ -4441,7 +4483,7 @@
         <v>1</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>10</v>
@@ -4470,7 +4512,7 @@
         <v>1</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I119" s="2" t="s">
         <v>10</v>
@@ -4499,7 +4541,7 @@
         <v>1</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>10</v>
@@ -4528,7 +4570,7 @@
         <v>1</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I121" s="2" t="s">
         <v>10</v>
@@ -4557,7 +4599,7 @@
         <v>1</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>0</v>
@@ -4586,7 +4628,7 @@
         <v>1</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>0</v>
@@ -4615,7 +4657,7 @@
         <v>1</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>0</v>
@@ -4644,7 +4686,7 @@
         <v>1</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I125" s="1" t="s">
         <v>0</v>
@@ -4673,7 +4715,7 @@
         <v>1</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I126" s="1" t="s">
         <v>0</v>
@@ -4702,7 +4744,7 @@
         <v>1</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I127" s="2" t="s">
         <v>10</v>
@@ -4731,7 +4773,7 @@
         <v>1</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I128" s="2" t="s">
         <v>10</v>
@@ -4760,7 +4802,7 @@
         <v>1</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I129" s="2" t="s">
         <v>10</v>
@@ -4789,7 +4831,7 @@
         <v>1</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I130" s="2" t="s">
         <v>10</v>
@@ -4818,7 +4860,7 @@
         <v>1</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I131" s="2" t="s">
         <v>10</v>
@@ -4847,7 +4889,7 @@
         <v>1</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>0</v>
@@ -4876,7 +4918,7 @@
         <v>1</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I133" s="1" t="s">
         <v>0</v>
@@ -4905,7 +4947,7 @@
         <v>1</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I134" s="1" t="s">
         <v>0</v>
@@ -4934,7 +4976,7 @@
         <v>1</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I135" s="1" t="s">
         <v>0</v>
@@ -4963,7 +5005,7 @@
         <v>1</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I136" s="1" t="s">
         <v>0</v>
@@ -4992,7 +5034,7 @@
         <v>1</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I137" s="1" t="s">
         <v>0</v>
@@ -5021,7 +5063,7 @@
         <v>1</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I138" s="1" t="s">
         <v>0</v>
@@ -5050,7 +5092,7 @@
         <v>1</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I139" s="1" t="s">
         <v>0</v>
@@ -5079,7 +5121,7 @@
         <v>1</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I140" s="1" t="s">
         <v>0</v>
@@ -5108,7 +5150,7 @@
         <v>1</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I141" s="1" t="s">
         <v>0</v>
@@ -5137,7 +5179,7 @@
         <v>1</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I142" s="1" t="s">
         <v>0</v>
@@ -5166,7 +5208,7 @@
         <v>1</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I143" s="1" t="s">
         <v>0</v>
@@ -5195,7 +5237,7 @@
         <v>1</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>0</v>
@@ -5205,7 +5247,9 @@
       <c r="A145" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B145" s="1"/>
+      <c r="B145" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C145" s="2" t="s">
         <v>40</v>
       </c>
@@ -5232,7 +5276,9 @@
       <c r="A146" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B146" s="1"/>
+      <c r="B146" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C146" s="2" t="s">
         <v>40</v>
       </c>
@@ -5278,7 +5324,7 @@
         <v>1</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I147" s="1" t="s">
         <v>0</v>
@@ -5307,7 +5353,7 @@
         <v>1</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>0</v>
@@ -5336,7 +5382,7 @@
         <v>1</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>0</v>
@@ -5365,7 +5411,7 @@
         <v>1</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>0</v>
@@ -5394,7 +5440,7 @@
         <v>1</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>0</v>
@@ -5404,7 +5450,9 @@
       <c r="A152" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B152" s="1"/>
+      <c r="B152" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C152" s="2" t="s">
         <v>38</v>
       </c>
@@ -5431,7 +5479,9 @@
       <c r="A153" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B153" s="1"/>
+      <c r="B153" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C153" s="2" t="s">
         <v>38</v>
       </c>
@@ -5477,7 +5527,7 @@
         <v>1</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I154" s="1" t="s">
         <v>0</v>
@@ -5506,7 +5556,7 @@
         <v>1</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I155" s="1" t="s">
         <v>0</v>
@@ -5535,7 +5585,7 @@
         <v>1</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I156" s="1" t="s">
         <v>0</v>
@@ -5564,7 +5614,7 @@
         <v>1</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I157" s="2" t="s">
         <v>10</v>
@@ -5593,7 +5643,7 @@
         <v>1</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I158" s="2" t="s">
         <v>10</v>
@@ -5622,7 +5672,7 @@
         <v>1</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I159" s="2" t="s">
         <v>37</v>
@@ -5651,7 +5701,7 @@
         <v>1</v>
       </c>
       <c r="H160" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I160" s="2" t="s">
         <v>10</v>
@@ -5680,7 +5730,7 @@
         <v>1</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I161" s="2" t="s">
         <v>10</v>
@@ -5709,7 +5759,7 @@
         <v>1</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I162" s="1" t="s">
         <v>0</v>
@@ -5738,7 +5788,7 @@
         <v>1</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I163" s="1" t="s">
         <v>0</v>
@@ -5767,7 +5817,7 @@
         <v>1</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I164" s="1" t="s">
         <v>0</v>
@@ -5796,7 +5846,7 @@
         <v>1</v>
       </c>
       <c r="H165" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I165" s="1" t="s">
         <v>0</v>
@@ -5807,7 +5857,7 @@
         <v>35</v>
       </c>
       <c r="B166" s="1">
-        <v>45826</v>
+        <v>45926</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>34</v>
@@ -5825,7 +5875,7 @@
         <v>1</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I166" s="1" t="s">
         <v>10</v>
@@ -5854,7 +5904,7 @@
         <v>1</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I167" s="1" t="s">
         <v>0</v>
@@ -5864,7 +5914,9 @@
       <c r="A168" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B168" s="1"/>
+      <c r="B168" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C168" s="2" t="s">
         <v>32</v>
       </c>
@@ -5910,7 +5962,7 @@
         <v>1</v>
       </c>
       <c r="H169" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I169" s="1" t="s">
         <v>0</v>
@@ -5920,7 +5972,9 @@
       <c r="A170" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B170" s="1"/>
+      <c r="B170" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C170" s="2" t="s">
         <v>32</v>
       </c>
@@ -5947,7 +6001,9 @@
       <c r="A171" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B171" s="1"/>
+      <c r="B171" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C171" s="2" t="s">
         <v>32</v>
       </c>
@@ -5993,7 +6049,7 @@
         <v>1</v>
       </c>
       <c r="H172" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I172" s="1" t="s">
         <v>0</v>
@@ -6022,7 +6078,7 @@
         <v>1</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I173" s="1" t="s">
         <v>0</v>
@@ -6051,7 +6107,7 @@
         <v>1</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I174" s="1" t="s">
         <v>0</v>
@@ -6080,7 +6136,7 @@
         <v>1</v>
       </c>
       <c r="H175" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I175" s="1" t="s">
         <v>0</v>
@@ -6109,7 +6165,7 @@
         <v>1</v>
       </c>
       <c r="H176" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I176" s="1" t="s">
         <v>0</v>
@@ -6138,7 +6194,7 @@
         <v>1</v>
       </c>
       <c r="H177" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I177" s="1" t="s">
         <v>0</v>
@@ -6167,7 +6223,7 @@
         <v>1</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I178" s="1" t="s">
         <v>0</v>
@@ -6196,7 +6252,7 @@
         <v>1</v>
       </c>
       <c r="H179" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I179" s="1" t="s">
         <v>0</v>
@@ -6225,7 +6281,7 @@
         <v>1</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I180" s="2" t="s">
         <v>10</v>
@@ -6254,7 +6310,7 @@
         <v>1</v>
       </c>
       <c r="H181" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I181" s="2" t="s">
         <v>10</v>
@@ -6283,7 +6339,7 @@
         <v>1</v>
       </c>
       <c r="H182" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I182" s="2" t="s">
         <v>28</v>
@@ -6312,7 +6368,7 @@
         <v>1</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I183" s="2" t="s">
         <v>16</v>
@@ -6341,7 +6397,7 @@
         <v>1</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I184" s="2" t="s">
         <v>27</v>
@@ -6370,7 +6426,7 @@
         <v>1</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I185" s="2" t="s">
         <v>26</v>
@@ -6399,7 +6455,7 @@
         <v>1</v>
       </c>
       <c r="H186" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I186" s="2" t="s">
         <v>24</v>
@@ -6428,7 +6484,7 @@
         <v>1</v>
       </c>
       <c r="H187" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I187" s="1" t="s">
         <v>0</v>
@@ -6457,7 +6513,7 @@
         <v>1</v>
       </c>
       <c r="H188" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I188" s="1" t="s">
         <v>0</v>
@@ -6486,7 +6542,7 @@
         <v>1</v>
       </c>
       <c r="H189" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I189" s="1" t="s">
         <v>0</v>
@@ -6515,7 +6571,7 @@
         <v>1</v>
       </c>
       <c r="H190" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I190" s="1" t="s">
         <v>0</v>
@@ -6544,7 +6600,7 @@
         <v>1</v>
       </c>
       <c r="H191" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I191" s="1" t="s">
         <v>0</v>
@@ -6573,7 +6629,7 @@
         <v>1</v>
       </c>
       <c r="H192" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I192" s="1" t="s">
         <v>0</v>
@@ -6602,7 +6658,7 @@
         <v>1</v>
       </c>
       <c r="H193" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I193" s="1" t="s">
         <v>0</v>
@@ -6631,7 +6687,7 @@
         <v>1</v>
       </c>
       <c r="H194" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I194" s="1" t="s">
         <v>0</v>
@@ -6660,7 +6716,7 @@
         <v>1</v>
       </c>
       <c r="H195" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I195" s="2" t="s">
         <v>10</v>
@@ -6689,7 +6745,7 @@
         <v>1</v>
       </c>
       <c r="H196" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I196" s="1" t="s">
         <v>0</v>
@@ -6718,7 +6774,7 @@
         <v>1</v>
       </c>
       <c r="H197" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I197" s="1" t="s">
         <v>0</v>
@@ -6747,7 +6803,7 @@
         <v>1</v>
       </c>
       <c r="H198" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I198" s="1" t="s">
         <v>0</v>
@@ -6776,7 +6832,7 @@
         <v>1</v>
       </c>
       <c r="H199" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I199" s="1" t="s">
         <v>0</v>
@@ -6805,7 +6861,7 @@
         <v>1</v>
       </c>
       <c r="H200" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I200" s="1" t="s">
         <v>0</v>
@@ -6834,7 +6890,7 @@
         <v>1</v>
       </c>
       <c r="H201" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I201" s="1" t="s">
         <v>0</v>
@@ -6845,7 +6901,7 @@
         <v>4</v>
       </c>
       <c r="B202" s="1">
-        <v>45924</v>
+        <v>45923</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>20</v>
@@ -6863,7 +6919,7 @@
         <v>1</v>
       </c>
       <c r="H202" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I202" s="1" t="s">
         <v>10</v>
@@ -6874,7 +6930,7 @@
         <v>4</v>
       </c>
       <c r="B203" s="1">
-        <v>45642</v>
+        <v>45597</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>20</v>
@@ -6892,7 +6948,7 @@
         <v>1</v>
       </c>
       <c r="H203" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I203" s="1" t="s">
         <v>0</v>
@@ -6921,7 +6977,7 @@
         <v>1</v>
       </c>
       <c r="H204" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I204" s="1" t="s">
         <v>10</v>
@@ -6932,7 +6988,7 @@
         <v>4</v>
       </c>
       <c r="B205" s="1">
-        <v>45924</v>
+        <v>45923</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>20</v>
@@ -6950,7 +7006,7 @@
         <v>1</v>
       </c>
       <c r="H205" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I205" s="1" t="s">
         <v>10</v>
@@ -6979,7 +7035,7 @@
         <v>1</v>
       </c>
       <c r="H206" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I206" s="1" t="s">
         <v>10</v>
@@ -7008,7 +7064,7 @@
         <v>1</v>
       </c>
       <c r="H207" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I207" s="2" t="s">
         <v>19</v>
@@ -7037,7 +7093,7 @@
         <v>1</v>
       </c>
       <c r="H208" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I208" s="2" t="s">
         <v>18</v>
@@ -7066,7 +7122,7 @@
         <v>1</v>
       </c>
       <c r="H209" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I209" s="2" t="s">
         <v>17</v>
@@ -7095,7 +7151,7 @@
         <v>1</v>
       </c>
       <c r="H210" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I210" s="2" t="s">
         <v>16</v>
@@ -7124,7 +7180,7 @@
         <v>1</v>
       </c>
       <c r="H211" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I211" s="2" t="s">
         <v>14</v>
@@ -7153,7 +7209,7 @@
         <v>1</v>
       </c>
       <c r="H212" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I212" s="1" t="s">
         <v>0</v>
@@ -7182,7 +7238,7 @@
         <v>1</v>
       </c>
       <c r="H213" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I213" s="1" t="s">
         <v>0</v>
@@ -7211,7 +7267,7 @@
         <v>1</v>
       </c>
       <c r="H214" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I214" s="1" t="s">
         <v>0</v>
@@ -7240,7 +7296,7 @@
         <v>1</v>
       </c>
       <c r="H215" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I215" s="1" t="s">
         <v>0</v>
@@ -7269,7 +7325,7 @@
         <v>1</v>
       </c>
       <c r="H216" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I216" s="1" t="s">
         <v>0</v>
@@ -7298,7 +7354,7 @@
         <v>1</v>
       </c>
       <c r="H217" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I217" s="1" t="s">
         <v>0</v>
@@ -7327,7 +7383,7 @@
         <v>1</v>
       </c>
       <c r="H218" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I218" s="1" t="s">
         <v>0</v>
@@ -7356,7 +7412,7 @@
         <v>1</v>
       </c>
       <c r="H219" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I219" s="1" t="s">
         <v>0</v>
@@ -7385,7 +7441,7 @@
         <v>1</v>
       </c>
       <c r="H220" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I220" s="1" t="s">
         <v>0</v>
@@ -7414,7 +7470,7 @@
         <v>1</v>
       </c>
       <c r="H221" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I221" s="1" t="s">
         <v>0</v>
@@ -7443,7 +7499,7 @@
         <v>1</v>
       </c>
       <c r="H222" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I222" s="1" t="s">
         <v>0</v>
@@ -7472,7 +7528,7 @@
         <v>1</v>
       </c>
       <c r="H223" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I223" s="1" t="s">
         <v>0</v>
@@ -7501,7 +7557,7 @@
         <v>1</v>
       </c>
       <c r="H224" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I224" s="1" t="s">
         <v>0</v>
@@ -7530,7 +7586,7 @@
         <v>1</v>
       </c>
       <c r="H225" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I225" s="1" t="s">
         <v>0</v>
@@ -7559,7 +7615,7 @@
         <v>1</v>
       </c>
       <c r="H226" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I226" s="1" t="s">
         <v>0</v>
@@ -7588,7 +7644,7 @@
         <v>1</v>
       </c>
       <c r="H227" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I227" s="1" t="s">
         <v>0</v>
@@ -7617,7 +7673,7 @@
         <v>1</v>
       </c>
       <c r="H228" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I228" s="1" t="s">
         <v>0</v>
@@ -7646,7 +7702,7 @@
         <v>1</v>
       </c>
       <c r="H229" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I229" s="2" t="s">
         <v>10</v>
@@ -7675,7 +7731,7 @@
         <v>1</v>
       </c>
       <c r="H230" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I230" s="1" t="s">
         <v>0</v>
@@ -7704,7 +7760,7 @@
         <v>1</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I231" s="1" t="s">
         <v>0</v>
@@ -7733,7 +7789,7 @@
         <v>1</v>
       </c>
       <c r="H232" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I232" s="1" t="s">
         <v>0</v>
@@ -7762,7 +7818,7 @@
         <v>1</v>
       </c>
       <c r="H233" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I233" s="1" t="s">
         <v>0</v>
@@ -7791,7 +7847,7 @@
         <v>1</v>
       </c>
       <c r="H234" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I234" s="1" t="s">
         <v>0</v>
@@ -7820,7 +7876,7 @@
         <v>1</v>
       </c>
       <c r="H235" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I235" s="1" t="s">
         <v>0</v>
@@ -7849,7 +7905,7 @@
         <v>1</v>
       </c>
       <c r="H236" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I236" s="8" t="s">
         <v>0</v>
@@ -7880,4 +7936,243 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54BAECB3-F31B-426D-96A4-E0BC1CD5DA1B}">
+  <dimension ref="D3:K14"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D3" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="G3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D4" s="14">
+        <v>2024</v>
+      </c>
+      <c r="E4" s="14">
+        <v>2025</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14">
+        <v>2024</v>
+      </c>
+      <c r="H4" s="14">
+        <v>2025</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14">
+        <v>2024</v>
+      </c>
+      <c r="K4" s="14">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="J5" t="b">
+        <f>G5=D5</f>
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <f>H5=E5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>14</v>
+      </c>
+      <c r="J6" t="b">
+        <f>G6=D6</f>
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <f t="shared" ref="K6:K14" si="0">H6=E6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="J7" t="b">
+        <f>G7=D7</f>
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
+      </c>
+      <c r="J8" t="b">
+        <f>G8=D8</f>
+        <v>1</v>
+      </c>
+      <c r="K8" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="J9" t="b">
+        <f>G9=D9</f>
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>31</v>
+      </c>
+      <c r="J10" t="b">
+        <f>G10=D10</f>
+        <v>0</v>
+      </c>
+      <c r="K10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>32</v>
+      </c>
+      <c r="H11">
+        <v>40</v>
+      </c>
+      <c r="J11" t="b">
+        <f>G11=D11</f>
+        <v>1</v>
+      </c>
+      <c r="K11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>36</v>
+      </c>
+      <c r="H12">
+        <v>36</v>
+      </c>
+      <c r="K12" t="b">
+        <f>H12=E12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>37</v>
+      </c>
+      <c r="H13">
+        <v>31</v>
+      </c>
+      <c r="K13" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remoção do botão filtro e Atualizar.
</commit_message>
<xml_diff>
--- a/Analise-de-substituicao-de-calliper.xlsx
+++ b/Analise-de-substituicao-de-calliper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de.ferreira\Desktop\dashboard-substituicao-calliper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAA4B9E-2949-4689-B828-639CA0A4177C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97A14F8-0300-4DEB-AE09-FD630E81B04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FA9E4268-8FE5-4DC5-93B3-4B3954182B74}"/>
   </bookViews>
@@ -436,10 +436,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1045,11 +1045,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B081B7-EA77-45F0-9C85-62DDCE899F30}">
-  <dimension ref="A1:M236"/>
+  <dimension ref="A1:L236"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1062,11 +1062,10 @@
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>78</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>61</v>
       </c>
@@ -1124,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>61</v>
       </c>
@@ -1153,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>61</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>61</v>
       </c>
@@ -1211,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -1240,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
@@ -1269,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>61</v>
       </c>
@@ -1298,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>61</v>
       </c>
@@ -1327,7 +1326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
@@ -1356,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
@@ -1384,9 +1383,9 @@
       <c r="I11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>61</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
@@ -1444,7 +1443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>61</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>61</v>
       </c>
@@ -1502,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
@@ -7926,7 +7925,7 @@
       <formula>$H2="By-passada"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H236" xr:uid="{4C4778BD-CA03-4ED1-9715-02EF6ED37E13}">
       <formula1>"Reparos substituidos, Informado por WEG, By-passada, Sem vazamento"</formula1>
     </dataValidation>
@@ -7953,34 +7952,34 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="E3" s="14"/>
+      <c r="G3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>2024</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>2025</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13">
         <v>2024</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <v>2025</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14">
+      <c r="I4" s="13"/>
+      <c r="J4" s="13">
         <v>2024</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="13">
         <v>2025</v>
       </c>
     </row>
@@ -8020,11 +8019,11 @@
         <v>14</v>
       </c>
       <c r="J6" t="b">
-        <f>G6=D6</f>
+        <f t="shared" ref="J6:J11" si="0">G6=D6</f>
         <v>1</v>
       </c>
       <c r="K6" t="b">
-        <f t="shared" ref="K6:K14" si="0">H6=E6</f>
+        <f t="shared" ref="K6:K14" si="1">H6=E6</f>
         <v>1</v>
       </c>
     </row>
@@ -8042,11 +8041,11 @@
         <v>3</v>
       </c>
       <c r="J7" t="b">
-        <f>G7=D7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K7" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8064,11 +8063,11 @@
         <v>9</v>
       </c>
       <c r="J8" t="b">
-        <f>G8=D8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8086,11 +8085,11 @@
         <v>10</v>
       </c>
       <c r="J9" t="b">
-        <f>G9=D9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K9" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -8108,11 +8107,11 @@
         <v>31</v>
       </c>
       <c r="J10" t="b">
-        <f>G10=D10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K10" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8124,11 +8123,11 @@
         <v>40</v>
       </c>
       <c r="J11" t="b">
-        <f>G11=D11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K11" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8152,7 +8151,7 @@
         <v>31</v>
       </c>
       <c r="K13" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8164,7 +8163,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Retirando sticky top-0 do titulo principal
</commit_message>
<xml_diff>
--- a/Analise-de-substituicao-de-calliper.xlsx
+++ b/Analise-de-substituicao-de-calliper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de.ferreira\Desktop\dashboard-substituicao-calliper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97A14F8-0300-4DEB-AE09-FD630E81B04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B529B9-1501-469B-A44F-8A3A0E325E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FA9E4268-8FE5-4DC5-93B3-4B3954182B74}"/>
   </bookViews>
@@ -1049,7 +1049,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
atualizacao de substituicao de callipers
</commit_message>
<xml_diff>
--- a/Analise-de-substituicao-de-calliper.xlsx
+++ b/Analise-de-substituicao-de-calliper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de.ferreira\Desktop\dashboard-substituicao-calliper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B529B9-1501-469B-A44F-8A3A0E325E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7FF9DE-57EA-40B1-8384-A2A7EF4298C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FA9E4268-8FE5-4DC5-93B3-4B3954182B74}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FA9E4268-8FE5-4DC5-93B3-4B3954182B74}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="86">
   <si>
     <t>-</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>SI-05</t>
-  </si>
-  <si>
-    <t>By-passada</t>
   </si>
   <si>
     <t>SI-42</t>
@@ -1049,7 +1046,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,42 +1064,42 @@
   <sheetData>
     <row r="1" spans="1:12" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="E1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7">
         <v>45798</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
@@ -1117,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>0</v>
@@ -1125,13 +1122,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1">
         <v>45820</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -1146,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>0</v>
@@ -1154,13 +1151,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1">
         <v>45888</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -1175,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>0</v>
@@ -1183,13 +1180,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1">
         <v>45888</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -1204,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>0</v>
@@ -1212,13 +1209,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1">
         <v>45820</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>2</v>
@@ -1233,7 +1230,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>0</v>
@@ -1241,13 +1238,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1">
         <v>45667</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -1262,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>0</v>
@@ -1270,13 +1267,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1">
         <v>45622</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>7</v>
@@ -1291,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>0</v>
@@ -1299,13 +1296,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1">
         <v>45761</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -1320,7 +1317,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>0</v>
@@ -1328,13 +1325,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1">
         <v>45761</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>5</v>
@@ -1349,7 +1346,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>0</v>
@@ -1357,13 +1354,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1">
         <v>45868</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
@@ -1378,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>0</v>
@@ -1387,13 +1384,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1">
         <v>45855</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -1408,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>16</v>
@@ -1416,13 +1413,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1">
         <v>45901</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
@@ -1437,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>10</v>
@@ -1445,13 +1442,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -1474,13 +1471,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>5</v>
@@ -1503,13 +1500,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1">
         <v>45901</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>2</v>
@@ -1524,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>10</v>
@@ -1532,13 +1529,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1">
         <v>45809</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -1553,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>0</v>
@@ -1561,13 +1558,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1">
         <v>45832</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
@@ -1582,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>0</v>
@@ -1590,13 +1587,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1">
         <v>45621</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -1611,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>0</v>
@@ -1619,13 +1616,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1">
         <v>45832</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>5</v>
@@ -1640,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>0</v>
@@ -1648,13 +1645,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="1">
         <v>45809</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>2</v>
@@ -1669,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>0</v>
@@ -1677,13 +1674,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1">
         <v>45649</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -1698,7 +1695,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>0</v>
@@ -1706,13 +1703,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1">
         <v>45712</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>7</v>
@@ -1727,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>0</v>
@@ -1735,13 +1732,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1">
         <v>45709</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
@@ -1756,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>0</v>
@@ -1764,13 +1761,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="1">
         <v>45709</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>5</v>
@@ -1785,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>0</v>
@@ -1793,13 +1790,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="1">
         <v>45712</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>2</v>
@@ -1814,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>0</v>
@@ -1822,13 +1819,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1">
         <v>45689</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>8</v>
@@ -1843,7 +1840,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>0</v>
@@ -1851,13 +1848,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1">
         <v>45447</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>7</v>
@@ -1872,7 +1869,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>0</v>
@@ -1880,13 +1877,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="1">
         <v>45689</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -1901,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>0</v>
@@ -1909,13 +1906,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="1">
         <v>45824</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
@@ -1930,7 +1927,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>0</v>
@@ -1938,13 +1935,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1">
         <v>45824</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>2</v>
@@ -1959,7 +1956,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>0</v>
@@ -1967,13 +1964,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="1">
         <v>45498</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>8</v>
@@ -1988,7 +1985,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>0</v>
@@ -1996,13 +1993,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1">
         <v>45933</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>7</v>
@@ -2017,7 +2014,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>10</v>
@@ -2025,13 +2022,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1">
         <v>45499</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>6</v>
@@ -2046,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>0</v>
@@ -2054,13 +2051,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1">
         <v>45833</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
@@ -2075,7 +2072,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>10</v>
@@ -2083,13 +2080,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1">
         <v>45833</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>2</v>
@@ -2104,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>10</v>
@@ -2112,13 +2109,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="1">
         <v>45930</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>8</v>
@@ -2133,7 +2130,7 @@
         <v>1</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>10</v>
@@ -2141,13 +2138,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1">
         <v>45929</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>7</v>
@@ -2162,7 +2159,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>10</v>
@@ -2170,13 +2167,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B39" s="1">
         <v>45930</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
@@ -2191,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>10</v>
@@ -2199,13 +2196,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1">
         <v>45930</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>5</v>
@@ -2220,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>10</v>
@@ -2228,13 +2225,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1">
         <v>45929</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>2</v>
@@ -2249,7 +2246,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>10</v>
@@ -2257,13 +2254,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B42" s="1">
         <v>45706</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>8</v>
@@ -2278,21 +2275,21 @@
         <v>1</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" s="1">
         <v>45660</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>7</v>
@@ -2307,21 +2304,21 @@
         <v>1</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B44" s="1">
         <v>45660</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>6</v>
@@ -2336,21 +2333,21 @@
         <v>1</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" s="1">
         <v>45856</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>5</v>
@@ -2365,21 +2362,21 @@
         <v>1</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="1">
         <v>45706</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>2</v>
@@ -2394,21 +2391,21 @@
         <v>1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B47" s="1">
         <v>45665</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>8</v>
@@ -2423,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>0</v>
@@ -2431,13 +2428,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48" s="1">
         <v>45665</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>7</v>
@@ -2452,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>0</v>
@@ -2460,13 +2457,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" s="1">
         <v>45870</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
@@ -2481,7 +2478,7 @@
         <v>1</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>0</v>
@@ -2489,13 +2486,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="1">
         <v>45870</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>5</v>
@@ -2510,7 +2507,7 @@
         <v>1</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>0</v>
@@ -2518,13 +2515,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51" s="1">
         <v>45870</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>2</v>
@@ -2539,7 +2536,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>0</v>
@@ -2547,13 +2544,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B52" s="1">
         <v>45862</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>8</v>
@@ -2568,7 +2565,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>0</v>
@@ -2576,13 +2573,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B53" s="1">
         <v>45623</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>7</v>
@@ -2597,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>0</v>
@@ -2605,13 +2602,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B54" s="1">
         <v>45936</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>6</v>
@@ -2626,7 +2623,7 @@
         <v>1</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>10</v>
@@ -2634,13 +2631,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B55" s="1">
         <v>45936</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>5</v>
@@ -2655,7 +2652,7 @@
         <v>1</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>10</v>
@@ -2663,13 +2660,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56" s="1">
         <v>45936</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>2</v>
@@ -2684,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>10</v>
@@ -2692,13 +2689,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>8</v>
@@ -2721,13 +2718,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B58" s="1">
         <v>45642</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>7</v>
@@ -2742,7 +2739,7 @@
         <v>1</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>0</v>
@@ -2750,13 +2747,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B59" s="1">
         <v>45853</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>6</v>
@@ -2771,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>0</v>
@@ -2779,13 +2776,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B60" s="1">
         <v>45723</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>5</v>
@@ -2800,7 +2797,7 @@
         <v>1</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>0</v>
@@ -2808,13 +2805,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B61" s="1">
         <v>45853</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>2</v>
@@ -2829,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>0</v>
@@ -2837,13 +2834,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B62" s="1">
         <v>45818</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>8</v>
@@ -2858,7 +2855,7 @@
         <v>1</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>0</v>
@@ -2866,13 +2863,13 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B63" s="1">
         <v>45776</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>7</v>
@@ -2887,7 +2884,7 @@
         <v>1</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>0</v>
@@ -2895,13 +2892,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B64" s="1">
         <v>45818</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
@@ -2916,7 +2913,7 @@
         <v>1</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>0</v>
@@ -2924,13 +2921,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B65" s="1">
         <v>45776</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>5</v>
@@ -2945,7 +2942,7 @@
         <v>1</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>0</v>
@@ -2953,13 +2950,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B66" s="1">
         <v>45894</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>2</v>
@@ -2974,7 +2971,7 @@
         <v>1</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>0</v>
@@ -2982,13 +2979,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B67" s="1">
         <v>45898</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>8</v>
@@ -3003,7 +3000,7 @@
         <v>1</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>0</v>
@@ -3011,13 +3008,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B68" s="1">
         <v>45898</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>7</v>
@@ -3032,7 +3029,7 @@
         <v>1</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>0</v>
@@ -3040,13 +3037,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B69" s="1">
         <v>45897</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>6</v>
@@ -3061,7 +3058,7 @@
         <v>1</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>0</v>
@@ -3069,13 +3066,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B70" s="1">
         <v>45897</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>5</v>
@@ -3090,7 +3087,7 @@
         <v>1</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>0</v>
@@ -3098,13 +3095,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B71" s="1">
         <v>45897</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>2</v>
@@ -3119,7 +3116,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>0</v>
@@ -3127,13 +3124,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B72" s="1">
         <v>45616</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>8</v>
@@ -3148,7 +3145,7 @@
         <v>1</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>0</v>
@@ -3156,13 +3153,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B73" s="1">
         <v>45624</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>7</v>
@@ -3177,7 +3174,7 @@
         <v>1</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>0</v>
@@ -3185,13 +3182,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B74" s="1">
         <v>45616</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>6</v>
@@ -3206,7 +3203,7 @@
         <v>1</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>0</v>
@@ -3214,13 +3211,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B75" s="1">
         <v>45846</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>5</v>
@@ -3235,7 +3232,7 @@
         <v>1</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>0</v>
@@ -3243,13 +3240,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B76" s="1">
         <v>45846</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>2</v>
@@ -3264,7 +3261,7 @@
         <v>1</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>0</v>
@@ -3272,13 +3269,13 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B77" s="1">
         <v>45895</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>8</v>
@@ -3293,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>0</v>
@@ -3301,13 +3298,13 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B78" s="1">
         <v>45895</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>7</v>
@@ -3322,7 +3319,7 @@
         <v>1</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>0</v>
@@ -3330,13 +3327,13 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>6</v>
@@ -3359,13 +3356,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>5</v>
@@ -3388,13 +3385,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>2</v>
@@ -3417,13 +3414,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B82" s="1">
         <v>45916</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>8</v>
@@ -3438,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>10</v>
@@ -3446,13 +3443,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B83" s="1">
         <v>45915</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>7</v>
@@ -3467,7 +3464,7 @@
         <v>1</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>10</v>
@@ -3475,13 +3472,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B84" s="1">
         <v>45916</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>6</v>
@@ -3496,7 +3493,7 @@
         <v>1</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>10</v>
@@ -3504,13 +3501,13 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B85" s="1">
         <v>45915</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>5</v>
@@ -3525,7 +3522,7 @@
         <v>1</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>10</v>
@@ -3533,13 +3530,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B86" s="1">
         <v>45916</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>2</v>
@@ -3554,7 +3551,7 @@
         <v>1</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>10</v>
@@ -3562,13 +3559,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B87" s="1">
         <v>45558</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>8</v>
@@ -3583,7 +3580,7 @@
         <v>1</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>0</v>
@@ -3591,13 +3588,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B88" s="1">
         <v>45565</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>7</v>
@@ -3612,7 +3609,7 @@
         <v>1</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>0</v>
@@ -3620,13 +3617,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B89" s="1">
         <v>45643</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>6</v>
@@ -3641,7 +3638,7 @@
         <v>1</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>0</v>
@@ -3649,13 +3646,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B90" s="1">
         <v>45702</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>5</v>
@@ -3670,7 +3667,7 @@
         <v>1</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>0</v>
@@ -3678,13 +3675,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B91" s="1">
         <v>45702</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>2</v>
@@ -3699,7 +3696,7 @@
         <v>1</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>0</v>
@@ -3707,13 +3704,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B92" s="1">
         <v>45845</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>8</v>
@@ -3728,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>0</v>
@@ -3736,13 +3733,13 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B93" s="1">
         <v>45869</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>7</v>
@@ -3757,7 +3754,7 @@
         <v>1</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>0</v>
@@ -3765,13 +3762,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B94" s="1">
         <v>45869</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>6</v>
@@ -3786,7 +3783,7 @@
         <v>1</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>0</v>
@@ -3794,13 +3791,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B95" s="1">
         <v>45845</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>5</v>
@@ -3815,7 +3812,7 @@
         <v>1</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>0</v>
@@ -3823,13 +3820,13 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B96" s="1">
         <v>45869</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>2</v>
@@ -3844,7 +3841,7 @@
         <v>1</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>0</v>
@@ -3852,13 +3849,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B97" s="1">
         <v>45884</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>8</v>
@@ -3873,7 +3870,7 @@
         <v>1</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>0</v>
@@ -3881,13 +3878,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B98" s="1">
         <v>45883</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>7</v>
@@ -3902,7 +3899,7 @@
         <v>1</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>0</v>
@@ -3910,13 +3907,13 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B99" s="1">
         <v>45884</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>6</v>
@@ -3931,7 +3928,7 @@
         <v>1</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>0</v>
@@ -3939,13 +3936,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B100" s="1">
         <v>45883</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>5</v>
@@ -3960,7 +3957,7 @@
         <v>1</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>0</v>
@@ -3968,13 +3965,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B101" s="1">
         <v>45883</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>2</v>
@@ -3989,7 +3986,7 @@
         <v>1</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>0</v>
@@ -3997,13 +3994,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B102" s="1">
         <v>45911</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>8</v>
@@ -4018,7 +4015,7 @@
         <v>1</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>10</v>
@@ -4026,13 +4023,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B103" s="1">
         <v>45866</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>7</v>
@@ -4047,7 +4044,7 @@
         <v>1</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>10</v>
@@ -4055,13 +4052,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B104" s="1">
         <v>45866</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>6</v>
@@ -4076,7 +4073,7 @@
         <v>1</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>10</v>
@@ -4084,13 +4081,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B105" s="1">
         <v>45911</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>5</v>
@@ -4105,7 +4102,7 @@
         <v>1</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>10</v>
@@ -4113,13 +4110,13 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B106" s="1">
         <v>45911</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>2</v>
@@ -4134,7 +4131,7 @@
         <v>1</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>10</v>
@@ -4142,13 +4139,13 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B107" s="1">
         <v>45835</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>8</v>
@@ -4163,7 +4160,7 @@
         <v>1</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>0</v>
@@ -4171,13 +4168,13 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B108" s="1">
         <v>45645</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>7</v>
@@ -4192,7 +4189,7 @@
         <v>1</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>0</v>
@@ -4200,13 +4197,13 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B109" s="1">
         <v>45835</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>6</v>
@@ -4221,7 +4218,7 @@
         <v>1</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>0</v>
@@ -4229,13 +4226,13 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B110" s="1">
         <v>45861</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>5</v>
@@ -4250,7 +4247,7 @@
         <v>1</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>0</v>
@@ -4258,13 +4255,13 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B111" s="1">
         <v>45861</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>2</v>
@@ -4279,7 +4276,7 @@
         <v>1</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>0</v>
@@ -4287,13 +4284,13 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B112" s="1">
         <v>45827</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>8</v>
@@ -4308,21 +4305,21 @@
         <v>1</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B113" s="1">
         <v>45652</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>7</v>
@@ -4337,21 +4334,21 @@
         <v>1</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B114" s="1">
         <v>45827</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>6</v>
@@ -4366,7 +4363,7 @@
         <v>1</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>10</v>
@@ -4374,13 +4371,13 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B115" s="1">
         <v>45903</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>5</v>
@@ -4395,7 +4392,7 @@
         <v>1</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>10</v>
@@ -4403,13 +4400,13 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B116" s="1">
         <v>45903</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>2</v>
@@ -4424,7 +4421,7 @@
         <v>1</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>10</v>
@@ -4432,13 +4429,13 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B117" s="1">
         <v>45918</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>8</v>
@@ -4453,7 +4450,7 @@
         <v>1</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>10</v>
@@ -4461,13 +4458,13 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B118" s="1">
         <v>45917</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>7</v>
@@ -4482,7 +4479,7 @@
         <v>1</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>10</v>
@@ -4490,13 +4487,13 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B119" s="1">
         <v>45918</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>6</v>
@@ -4511,7 +4508,7 @@
         <v>1</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I119" s="2" t="s">
         <v>10</v>
@@ -4519,13 +4516,13 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B120" s="1">
         <v>45917</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>5</v>
@@ -4540,7 +4537,7 @@
         <v>1</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>10</v>
@@ -4548,13 +4545,13 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B121" s="1">
         <v>45918</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>2</v>
@@ -4569,7 +4566,7 @@
         <v>1</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I121" s="2" t="s">
         <v>10</v>
@@ -4577,13 +4574,13 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B122" s="1">
         <v>45817</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>8</v>
@@ -4598,7 +4595,7 @@
         <v>1</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>0</v>
@@ -4606,13 +4603,13 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B123" s="1">
         <v>45817</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>7</v>
@@ -4627,7 +4624,7 @@
         <v>1</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>0</v>
@@ -4635,13 +4632,13 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B124" s="1">
         <v>45887</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>6</v>
@@ -4656,7 +4653,7 @@
         <v>1</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>0</v>
@@ -4664,13 +4661,13 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B125" s="1">
         <v>45887</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>5</v>
@@ -4685,7 +4682,7 @@
         <v>1</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I125" s="1" t="s">
         <v>0</v>
@@ -4693,13 +4690,13 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B126" s="1">
         <v>45887</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>2</v>
@@ -4714,7 +4711,7 @@
         <v>1</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I126" s="1" t="s">
         <v>0</v>
@@ -4722,13 +4719,13 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B127" s="1">
         <v>45909</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>8</v>
@@ -4743,7 +4740,7 @@
         <v>1</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I127" s="2" t="s">
         <v>10</v>
@@ -4751,13 +4748,13 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B128" s="1">
         <v>45909</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>7</v>
@@ -4772,7 +4769,7 @@
         <v>1</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I128" s="2" t="s">
         <v>10</v>
@@ -4780,13 +4777,13 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B129" s="1">
         <v>45910</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>6</v>
@@ -4801,7 +4798,7 @@
         <v>1</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I129" s="2" t="s">
         <v>10</v>
@@ -4809,13 +4806,13 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B130" s="1">
         <v>45910</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>5</v>
@@ -4830,7 +4827,7 @@
         <v>1</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I130" s="2" t="s">
         <v>10</v>
@@ -4838,13 +4835,13 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B131" s="1">
         <v>45910</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>2</v>
@@ -4859,7 +4856,7 @@
         <v>1</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I131" s="2" t="s">
         <v>10</v>
@@ -4867,13 +4864,13 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B132" s="1">
         <v>45896</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>8</v>
@@ -4888,7 +4885,7 @@
         <v>1</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>0</v>
@@ -4896,13 +4893,13 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B133" s="1">
         <v>45790</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>7</v>
@@ -4917,7 +4914,7 @@
         <v>1</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I133" s="1" t="s">
         <v>0</v>
@@ -4925,13 +4922,13 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B134" s="1">
         <v>45834</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>6</v>
@@ -4946,7 +4943,7 @@
         <v>1</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I134" s="1" t="s">
         <v>0</v>
@@ -4954,13 +4951,13 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B135" s="1">
         <v>45834</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>5</v>
@@ -4975,7 +4972,7 @@
         <v>1</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I135" s="1" t="s">
         <v>0</v>
@@ -4983,13 +4980,13 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B136" s="1">
         <v>45896</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>2</v>
@@ -5004,7 +5001,7 @@
         <v>1</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I136" s="1" t="s">
         <v>0</v>
@@ -5012,13 +5009,13 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B137" s="1">
         <v>45705</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>8</v>
@@ -5033,7 +5030,7 @@
         <v>1</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I137" s="1" t="s">
         <v>0</v>
@@ -5041,13 +5038,13 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B138" s="1">
         <v>45560</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>7</v>
@@ -5062,7 +5059,7 @@
         <v>1</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I138" s="1" t="s">
         <v>0</v>
@@ -5070,13 +5067,13 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B139" s="1">
         <v>45705</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>6</v>
@@ -5091,7 +5088,7 @@
         <v>1</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I139" s="1" t="s">
         <v>0</v>
@@ -5099,13 +5096,13 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B140" s="1">
         <v>45785</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>5</v>
@@ -5120,7 +5117,7 @@
         <v>1</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I140" s="1" t="s">
         <v>0</v>
@@ -5128,13 +5125,13 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B141" s="1">
         <v>45785</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>2</v>
@@ -5149,7 +5146,7 @@
         <v>1</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I141" s="1" t="s">
         <v>0</v>
@@ -5157,13 +5154,13 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B142" s="1">
         <v>45852</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>8</v>
@@ -5178,7 +5175,7 @@
         <v>1</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I142" s="1" t="s">
         <v>0</v>
@@ -5186,13 +5183,13 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B143" s="1">
         <v>45646</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>7</v>
@@ -5207,7 +5204,7 @@
         <v>1</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I143" s="1" t="s">
         <v>0</v>
@@ -5215,13 +5212,13 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B144" s="1">
         <v>45852</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>6</v>
@@ -5236,7 +5233,7 @@
         <v>1</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>0</v>
@@ -5244,13 +5241,13 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>5</v>
@@ -5273,13 +5270,13 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>2</v>
@@ -5302,13 +5299,13 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B147" s="1">
         <v>45555</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>8</v>
@@ -5323,7 +5320,7 @@
         <v>1</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I147" s="1" t="s">
         <v>0</v>
@@ -5331,13 +5328,13 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B148" s="1">
         <v>45647</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>7</v>
@@ -5352,7 +5349,7 @@
         <v>1</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>0</v>
@@ -5360,13 +5357,13 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B149" s="1">
         <v>45647</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>6</v>
@@ -5381,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>0</v>
@@ -5389,13 +5386,13 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B150" s="1">
         <v>45342</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>5</v>
@@ -5410,7 +5407,7 @@
         <v>1</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>0</v>
@@ -5418,13 +5415,13 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B151" s="1">
         <v>45342</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>2</v>
@@ -5439,7 +5436,7 @@
         <v>1</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>0</v>
@@ -5447,71 +5444,71 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="B152" s="1">
+        <v>45953</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E152" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F152" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G152" s="1" t="s">
-        <v>0</v>
+      <c r="E152" s="3">
+        <v>45953</v>
+      </c>
+      <c r="F152" s="3">
+        <v>45953</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="B153" s="1">
+        <v>45953</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E153" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>0</v>
+      <c r="E153" s="3">
+        <v>45953</v>
+      </c>
+      <c r="F153" s="3">
+        <v>45953</v>
+      </c>
+      <c r="G153" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B154" s="1">
         <v>45727</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>6</v>
@@ -5526,21 +5523,21 @@
         <v>1</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B155" s="1">
         <v>45860</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>5</v>
@@ -5555,21 +5552,21 @@
         <v>1</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B156" s="1">
         <v>45860</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>2</v>
@@ -5584,21 +5581,21 @@
         <v>1</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B157" s="1">
         <v>45908</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>8</v>
@@ -5613,7 +5610,7 @@
         <v>1</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I157" s="2" t="s">
         <v>10</v>
@@ -5621,13 +5618,13 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B158" s="1">
         <v>45503</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>7</v>
@@ -5642,7 +5639,7 @@
         <v>1</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I158" s="2" t="s">
         <v>10</v>
@@ -5650,13 +5647,13 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B159" s="1">
         <v>45825</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>6</v>
@@ -5671,21 +5668,21 @@
         <v>1</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B160" s="1">
         <v>45825</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>5</v>
@@ -5700,7 +5697,7 @@
         <v>1</v>
       </c>
       <c r="H160" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I160" s="2" t="s">
         <v>10</v>
@@ -5708,13 +5705,13 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B161" s="1">
         <v>45908</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>2</v>
@@ -5729,7 +5726,7 @@
         <v>1</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I161" s="2" t="s">
         <v>10</v>
@@ -5737,13 +5734,13 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B162" s="1">
         <v>45666</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>8</v>
@@ -5758,7 +5755,7 @@
         <v>1</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I162" s="1" t="s">
         <v>0</v>
@@ -5766,13 +5763,13 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B163" s="1">
         <v>45666</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>7</v>
@@ -5787,7 +5784,7 @@
         <v>1</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I163" s="1" t="s">
         <v>0</v>
@@ -5795,13 +5792,13 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B164" s="1">
         <v>45826</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>6</v>
@@ -5816,7 +5813,7 @@
         <v>1</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I164" s="1" t="s">
         <v>0</v>
@@ -5824,13 +5821,13 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B165" s="1">
         <v>45826</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>5</v>
@@ -5845,7 +5842,7 @@
         <v>1</v>
       </c>
       <c r="H165" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I165" s="1" t="s">
         <v>0</v>
@@ -5853,13 +5850,13 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B166" s="1">
         <v>45926</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>2</v>
@@ -5874,7 +5871,7 @@
         <v>1</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I166" s="1" t="s">
         <v>10</v>
@@ -5903,18 +5900,18 @@
         <v>1</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B168" s="1" t="s">
-        <v>0</v>
+      <c r="B168" s="1">
+        <v>45891</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>32</v>
@@ -5922,20 +5919,20 @@
       <c r="D168" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E168" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F168" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G168" s="1" t="s">
-        <v>0</v>
+      <c r="E168" s="3">
+        <v>45891</v>
+      </c>
+      <c r="F168" s="3">
+        <v>45891</v>
+      </c>
+      <c r="G168" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
@@ -5961,18 +5958,18 @@
         <v>1</v>
       </c>
       <c r="H169" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B170" s="1" t="s">
-        <v>0</v>
+      <c r="B170" s="1">
+        <v>45891</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>32</v>
@@ -5980,28 +5977,28 @@
       <c r="D170" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E170" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F170" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G170" s="1" t="s">
-        <v>0</v>
+      <c r="E170" s="3">
+        <v>45891</v>
+      </c>
+      <c r="F170" s="3">
+        <v>45891</v>
+      </c>
+      <c r="G170" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H170" s="2" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B171" s="1" t="s">
-        <v>0</v>
+      <c r="B171" s="1">
+        <v>45891</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>32</v>
@@ -6009,20 +6006,20 @@
       <c r="D171" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E171" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F171" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G171" s="1" t="s">
-        <v>0</v>
+      <c r="E171" s="3">
+        <v>45891</v>
+      </c>
+      <c r="F171" s="3">
+        <v>45891</v>
+      </c>
+      <c r="G171" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H171" s="2" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
@@ -6048,7 +6045,7 @@
         <v>1</v>
       </c>
       <c r="H172" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I172" s="1" t="s">
         <v>0</v>
@@ -6077,7 +6074,7 @@
         <v>1</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I173" s="1" t="s">
         <v>0</v>
@@ -6106,7 +6103,7 @@
         <v>1</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I174" s="1" t="s">
         <v>0</v>
@@ -6135,7 +6132,7 @@
         <v>1</v>
       </c>
       <c r="H175" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I175" s="1" t="s">
         <v>0</v>
@@ -6164,7 +6161,7 @@
         <v>1</v>
       </c>
       <c r="H176" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I176" s="1" t="s">
         <v>0</v>
@@ -6193,7 +6190,7 @@
         <v>1</v>
       </c>
       <c r="H177" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I177" s="1" t="s">
         <v>0</v>
@@ -6222,7 +6219,7 @@
         <v>1</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I178" s="1" t="s">
         <v>0</v>
@@ -6251,7 +6248,7 @@
         <v>1</v>
       </c>
       <c r="H179" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I179" s="1" t="s">
         <v>0</v>
@@ -6280,7 +6277,7 @@
         <v>1</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I180" s="2" t="s">
         <v>10</v>
@@ -6309,7 +6306,7 @@
         <v>1</v>
       </c>
       <c r="H181" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I181" s="2" t="s">
         <v>10</v>
@@ -6338,7 +6335,7 @@
         <v>1</v>
       </c>
       <c r="H182" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I182" s="2" t="s">
         <v>28</v>
@@ -6367,7 +6364,7 @@
         <v>1</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I183" s="2" t="s">
         <v>16</v>
@@ -6396,7 +6393,7 @@
         <v>1</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I184" s="2" t="s">
         <v>27</v>
@@ -6425,7 +6422,7 @@
         <v>1</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I185" s="2" t="s">
         <v>26</v>
@@ -6454,7 +6451,7 @@
         <v>1</v>
       </c>
       <c r="H186" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I186" s="2" t="s">
         <v>24</v>
@@ -6483,7 +6480,7 @@
         <v>1</v>
       </c>
       <c r="H187" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I187" s="1" t="s">
         <v>0</v>
@@ -6512,7 +6509,7 @@
         <v>1</v>
       </c>
       <c r="H188" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I188" s="1" t="s">
         <v>0</v>
@@ -6541,7 +6538,7 @@
         <v>1</v>
       </c>
       <c r="H189" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I189" s="1" t="s">
         <v>0</v>
@@ -6570,7 +6567,7 @@
         <v>1</v>
       </c>
       <c r="H190" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I190" s="1" t="s">
         <v>0</v>
@@ -6599,7 +6596,7 @@
         <v>1</v>
       </c>
       <c r="H191" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I191" s="1" t="s">
         <v>0</v>
@@ -6628,7 +6625,7 @@
         <v>1</v>
       </c>
       <c r="H192" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I192" s="1" t="s">
         <v>0</v>
@@ -6657,7 +6654,7 @@
         <v>1</v>
       </c>
       <c r="H193" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I193" s="1" t="s">
         <v>0</v>
@@ -6686,7 +6683,7 @@
         <v>1</v>
       </c>
       <c r="H194" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I194" s="1" t="s">
         <v>0</v>
@@ -6715,7 +6712,7 @@
         <v>1</v>
       </c>
       <c r="H195" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I195" s="2" t="s">
         <v>10</v>
@@ -6744,7 +6741,7 @@
         <v>1</v>
       </c>
       <c r="H196" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I196" s="1" t="s">
         <v>0</v>
@@ -6773,7 +6770,7 @@
         <v>1</v>
       </c>
       <c r="H197" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I197" s="1" t="s">
         <v>0</v>
@@ -6802,7 +6799,7 @@
         <v>1</v>
       </c>
       <c r="H198" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I198" s="1" t="s">
         <v>0</v>
@@ -6831,7 +6828,7 @@
         <v>1</v>
       </c>
       <c r="H199" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I199" s="1" t="s">
         <v>0</v>
@@ -6860,7 +6857,7 @@
         <v>1</v>
       </c>
       <c r="H200" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I200" s="1" t="s">
         <v>0</v>
@@ -6889,7 +6886,7 @@
         <v>1</v>
       </c>
       <c r="H201" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I201" s="1" t="s">
         <v>0</v>
@@ -6918,7 +6915,7 @@
         <v>1</v>
       </c>
       <c r="H202" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I202" s="1" t="s">
         <v>10</v>
@@ -6947,7 +6944,7 @@
         <v>1</v>
       </c>
       <c r="H203" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I203" s="1" t="s">
         <v>0</v>
@@ -6976,7 +6973,7 @@
         <v>1</v>
       </c>
       <c r="H204" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I204" s="1" t="s">
         <v>10</v>
@@ -7005,7 +7002,7 @@
         <v>1</v>
       </c>
       <c r="H205" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I205" s="1" t="s">
         <v>10</v>
@@ -7034,7 +7031,7 @@
         <v>1</v>
       </c>
       <c r="H206" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I206" s="1" t="s">
         <v>10</v>
@@ -7063,7 +7060,7 @@
         <v>1</v>
       </c>
       <c r="H207" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I207" s="2" t="s">
         <v>19</v>
@@ -7092,7 +7089,7 @@
         <v>1</v>
       </c>
       <c r="H208" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I208" s="2" t="s">
         <v>18</v>
@@ -7121,7 +7118,7 @@
         <v>1</v>
       </c>
       <c r="H209" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I209" s="2" t="s">
         <v>17</v>
@@ -7150,7 +7147,7 @@
         <v>1</v>
       </c>
       <c r="H210" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I210" s="2" t="s">
         <v>16</v>
@@ -7179,7 +7176,7 @@
         <v>1</v>
       </c>
       <c r="H211" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I211" s="2" t="s">
         <v>14</v>
@@ -7208,7 +7205,7 @@
         <v>1</v>
       </c>
       <c r="H212" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I212" s="1" t="s">
         <v>0</v>
@@ -7237,7 +7234,7 @@
         <v>1</v>
       </c>
       <c r="H213" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I213" s="1" t="s">
         <v>0</v>
@@ -7266,7 +7263,7 @@
         <v>1</v>
       </c>
       <c r="H214" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I214" s="1" t="s">
         <v>0</v>
@@ -7295,7 +7292,7 @@
         <v>1</v>
       </c>
       <c r="H215" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I215" s="1" t="s">
         <v>0</v>
@@ -7324,7 +7321,7 @@
         <v>1</v>
       </c>
       <c r="H216" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I216" s="1" t="s">
         <v>0</v>
@@ -7353,7 +7350,7 @@
         <v>1</v>
       </c>
       <c r="H217" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I217" s="1" t="s">
         <v>0</v>
@@ -7382,7 +7379,7 @@
         <v>1</v>
       </c>
       <c r="H218" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I218" s="1" t="s">
         <v>0</v>
@@ -7411,7 +7408,7 @@
         <v>1</v>
       </c>
       <c r="H219" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I219" s="1" t="s">
         <v>0</v>
@@ -7440,7 +7437,7 @@
         <v>1</v>
       </c>
       <c r="H220" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I220" s="1" t="s">
         <v>0</v>
@@ -7469,7 +7466,7 @@
         <v>1</v>
       </c>
       <c r="H221" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I221" s="1" t="s">
         <v>0</v>
@@ -7498,7 +7495,7 @@
         <v>1</v>
       </c>
       <c r="H222" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I222" s="1" t="s">
         <v>0</v>
@@ -7527,7 +7524,7 @@
         <v>1</v>
       </c>
       <c r="H223" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I223" s="1" t="s">
         <v>0</v>
@@ -7556,7 +7553,7 @@
         <v>1</v>
       </c>
       <c r="H224" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I224" s="1" t="s">
         <v>0</v>
@@ -7585,7 +7582,7 @@
         <v>1</v>
       </c>
       <c r="H225" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I225" s="1" t="s">
         <v>0</v>
@@ -7614,7 +7611,7 @@
         <v>1</v>
       </c>
       <c r="H226" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I226" s="1" t="s">
         <v>0</v>
@@ -7643,7 +7640,7 @@
         <v>1</v>
       </c>
       <c r="H227" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I227" s="1" t="s">
         <v>0</v>
@@ -7672,7 +7669,7 @@
         <v>1</v>
       </c>
       <c r="H228" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I228" s="1" t="s">
         <v>0</v>
@@ -7701,7 +7698,7 @@
         <v>1</v>
       </c>
       <c r="H229" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I229" s="2" t="s">
         <v>10</v>
@@ -7730,7 +7727,7 @@
         <v>1</v>
       </c>
       <c r="H230" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I230" s="1" t="s">
         <v>0</v>
@@ -7759,7 +7756,7 @@
         <v>1</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I231" s="1" t="s">
         <v>0</v>
@@ -7788,7 +7785,7 @@
         <v>1</v>
       </c>
       <c r="H232" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I232" s="1" t="s">
         <v>0</v>
@@ -7817,7 +7814,7 @@
         <v>1</v>
       </c>
       <c r="H233" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I233" s="1" t="s">
         <v>0</v>
@@ -7846,7 +7843,7 @@
         <v>1</v>
       </c>
       <c r="H234" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I234" s="1" t="s">
         <v>0</v>
@@ -7875,7 +7872,7 @@
         <v>1</v>
       </c>
       <c r="H235" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I235" s="1" t="s">
         <v>0</v>
@@ -7904,7 +7901,7 @@
         <v>1</v>
       </c>
       <c r="H236" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I236" s="8" t="s">
         <v>0</v>
@@ -7953,11 +7950,11 @@
   <sheetData>
     <row r="3" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D3" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H3" s="14"/>
     </row>

</xml_diff>

<commit_message>
Atulaizando Lista de Callipers by-passado
</commit_message>
<xml_diff>
--- a/Analise-de-substituicao-de-calliper.xlsx
+++ b/Analise-de-substituicao-de-calliper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de.ferreira\Desktop\dashboard-substituicao-calliper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4468D2C-3ADC-4D55-BB3A-89D31D96C106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809EE1C7-43D8-4B16-8CF8-94F37C0C4909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FA9E4268-8FE5-4DC5-93B3-4B3954182B74}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="86">
   <si>
     <t>-</t>
   </si>
@@ -2691,8 +2691,9 @@
       <c r="A57" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>0</v>
+      <c r="B57" s="1">
+        <f>Tabela134[[#This Row],[SUBSTITUICAO DO ORING]]</f>
+        <v>45957</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>58</v>
@@ -2700,20 +2701,20 @@
       <c r="D57" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>0</v>
+      <c r="E57" s="3">
+        <v>45957</v>
+      </c>
+      <c r="F57" s="3">
+        <v>45957</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -5243,8 +5244,8 @@
       <c r="A145" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>0</v>
+      <c r="B145" s="1">
+        <v>45904</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>39</v>
@@ -5252,28 +5253,28 @@
       <c r="D145" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E145" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F145" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>0</v>
+      <c r="E145" s="3">
+        <v>45904</v>
+      </c>
+      <c r="F145" s="3">
+        <v>45904</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>0</v>
+      <c r="B146" s="1">
+        <v>45772</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>39</v>
@@ -5281,20 +5282,20 @@
       <c r="D146" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E146" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F146" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G146" s="1" t="s">
-        <v>0</v>
+      <c r="E146" s="3">
+        <v>45772</v>
+      </c>
+      <c r="F146" s="3">
+        <v>45772</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
retirando a SI-12 das máquinas com pendencia.
</commit_message>
<xml_diff>
--- a/Analise-de-substituicao-de-calliper.xlsx
+++ b/Analise-de-substituicao-de-calliper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de.ferreira\Desktop\dashboard-substituicao-calliper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD6A918-3557-4761-9949-7754668F1E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF27786A-231E-4F9F-8EEB-B02306AE8601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="19090" yWindow="-100" windowWidth="19420" windowHeight="10300" xr2:uid="{FA9E4268-8FE5-4DC5-93B3-4B3954182B74}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FA9E4268-8FE5-4DC5-93B3-4B3954182B74}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="87">
   <si>
     <t>-</t>
   </si>
@@ -1049,8 +1049,8 @@
   <dimension ref="A1:L242"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3334,7 +3334,7 @@
       <c r="A79" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="1">
         <f>Tabela134[[#This Row],[SUBSTITUICAO DO ORING]]</f>
         <v>45905</v>
       </c>
@@ -3364,8 +3364,8 @@
       <c r="A80" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="3" t="s">
-        <v>0</v>
+      <c r="B80" s="1">
+        <v>45973</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>54</v>
@@ -3373,27 +3373,27 @@
       <c r="D80" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E80" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>0</v>
+      <c r="E80" s="3">
+        <v>45973</v>
+      </c>
+      <c r="F80" s="3">
+        <v>45973</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>0</v>
+        <v>79</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="1">
         <f>Tabela134[[#This Row],[SUBSTITUICAO DO ORING]]</f>
         <v>45905</v>
       </c>

</xml_diff>

<commit_message>
Update database with inspection information
</commit_message>
<xml_diff>
--- a/Analise-de-substituicao-de-calliper.xlsx
+++ b/Analise-de-substituicao-de-calliper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de.ferreira\Desktop\dashboard-substituicao-calliper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF27786A-231E-4F9F-8EEB-B02306AE8601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25E243B-EE69-4C0D-B698-9CD7A67C5F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FA9E4268-8FE5-4DC5-93B3-4B3954182B74}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="85">
   <si>
     <t>-</t>
   </si>
@@ -132,9 +132,6 @@
     <t>SI-06</t>
   </si>
   <si>
-    <t>Sem vazamento</t>
-  </si>
-  <si>
     <t>SI-05</t>
   </si>
   <si>
@@ -295,9 +292,6 @@
   </si>
   <si>
     <t>No codigo</t>
-  </si>
-  <si>
-    <t>troca de oring</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1044,7 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
+      <selection pane="bottomLeft" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,42 +1062,42 @@
   <sheetData>
     <row r="1" spans="1:12" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="E1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="7">
         <v>45798</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
@@ -1118,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>0</v>
@@ -1126,13 +1120,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="1">
         <v>45820</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -1147,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>0</v>
@@ -1155,13 +1149,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1">
         <v>45888</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -1176,7 +1170,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>0</v>
@@ -1184,13 +1178,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1">
         <v>45888</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -1205,7 +1199,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>0</v>
@@ -1213,13 +1207,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1">
         <v>45820</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>2</v>
@@ -1234,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>0</v>
@@ -1242,13 +1236,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1">
         <v>45667</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -1263,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>0</v>
@@ -1271,13 +1265,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1">
         <v>45622</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>7</v>
@@ -1292,7 +1286,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>0</v>
@@ -1300,13 +1294,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="1">
         <v>45761</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -1321,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>0</v>
@@ -1329,13 +1323,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1">
         <v>45761</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>5</v>
@@ -1350,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>0</v>
@@ -1358,13 +1352,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1">
         <v>45868</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
@@ -1379,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>0</v>
@@ -1388,13 +1382,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1">
         <v>45855</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -1409,7 +1403,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>16</v>
@@ -1417,13 +1411,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1">
         <v>45901</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
@@ -1438,7 +1432,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>10</v>
@@ -1446,28 +1440,28 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45902</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>0</v>
+      <c r="E14" s="3">
+        <v>45902</v>
+      </c>
+      <c r="F14" s="3">
+        <v>45902</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>0</v>
@@ -1475,28 +1469,28 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45902</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>0</v>
+      <c r="E15" s="3">
+        <v>45902</v>
+      </c>
+      <c r="F15" s="3">
+        <v>45902</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>0</v>
@@ -1504,13 +1498,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1">
         <v>45901</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>2</v>
@@ -1525,7 +1519,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>10</v>
@@ -1533,13 +1527,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1">
         <v>45809</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -1554,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>0</v>
@@ -1562,13 +1556,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1">
         <v>45832</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
@@ -1583,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>0</v>
@@ -1591,13 +1585,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1">
         <v>45621</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -1612,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>0</v>
@@ -1620,13 +1614,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1">
         <v>45832</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>5</v>
@@ -1641,7 +1635,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>0</v>
@@ -1649,13 +1643,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="1">
         <v>45809</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>2</v>
@@ -1670,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>0</v>
@@ -1678,13 +1672,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1">
         <v>45649</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -1699,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>0</v>
@@ -1707,13 +1701,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="1">
         <v>45712</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>7</v>
@@ -1728,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>0</v>
@@ -1736,13 +1730,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="1">
         <v>45709</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
@@ -1757,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>0</v>
@@ -1765,13 +1759,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1">
         <v>45709</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>5</v>
@@ -1786,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>0</v>
@@ -1794,13 +1788,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1">
         <v>45712</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>2</v>
@@ -1815,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>0</v>
@@ -1823,13 +1817,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1">
         <v>45689</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>8</v>
@@ -1844,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>0</v>
@@ -1852,13 +1846,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="1">
         <v>45447</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>7</v>
@@ -1873,7 +1867,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>0</v>
@@ -1881,13 +1875,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1">
         <v>45689</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -1902,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>0</v>
@@ -1910,13 +1904,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1">
         <v>45824</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
@@ -1931,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>0</v>
@@ -1939,13 +1933,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="1">
         <v>45824</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>2</v>
@@ -1960,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>0</v>
@@ -1968,13 +1962,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1">
         <v>45498</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>8</v>
@@ -1989,7 +1983,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>0</v>
@@ -1997,13 +1991,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1">
         <v>45933</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>7</v>
@@ -2018,7 +2012,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>10</v>
@@ -2026,13 +2020,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="1">
         <v>45499</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>6</v>
@@ -2047,7 +2041,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>0</v>
@@ -2055,13 +2049,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="1">
         <v>45833</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
@@ -2076,7 +2070,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>10</v>
@@ -2084,13 +2078,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="1">
         <v>45833</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>2</v>
@@ -2105,7 +2099,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>10</v>
@@ -2113,13 +2107,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" s="1">
         <v>45930</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>8</v>
@@ -2134,7 +2128,7 @@
         <v>1</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>10</v>
@@ -2142,13 +2136,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" s="1">
         <v>45929</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>7</v>
@@ -2163,7 +2157,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>10</v>
@@ -2171,13 +2165,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="1">
         <v>45930</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
@@ -2192,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>10</v>
@@ -2200,13 +2194,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1">
         <v>45930</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>5</v>
@@ -2221,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>10</v>
@@ -2229,13 +2223,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" s="1">
         <v>45929</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>2</v>
@@ -2250,7 +2244,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>10</v>
@@ -2258,13 +2252,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" s="1">
         <v>45706</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>8</v>
@@ -2279,21 +2273,21 @@
         <v>1</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" s="1">
         <v>45660</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>7</v>
@@ -2308,21 +2302,21 @@
         <v>1</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44" s="1">
         <v>45660</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>6</v>
@@ -2337,21 +2331,21 @@
         <v>1</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B45" s="1">
         <v>45856</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>5</v>
@@ -2366,21 +2360,21 @@
         <v>1</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" s="1">
         <v>45706</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>2</v>
@@ -2395,21 +2389,21 @@
         <v>1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47" s="1">
         <v>45665</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>8</v>
@@ -2424,7 +2418,7 @@
         <v>1</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>0</v>
@@ -2432,13 +2426,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" s="1">
         <v>45665</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>7</v>
@@ -2453,7 +2447,7 @@
         <v>1</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>0</v>
@@ -2461,13 +2455,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" s="1">
         <v>45870</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
@@ -2482,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>0</v>
@@ -2490,13 +2484,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" s="1">
         <v>45870</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>5</v>
@@ -2511,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>0</v>
@@ -2519,13 +2513,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" s="1">
         <v>45870</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>2</v>
@@ -2540,7 +2534,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>0</v>
@@ -2548,13 +2542,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52" s="1">
         <v>45862</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>8</v>
@@ -2569,7 +2563,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>0</v>
@@ -2577,13 +2571,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" s="1">
         <v>45623</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>7</v>
@@ -2598,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>0</v>
@@ -2606,13 +2600,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54" s="1">
         <v>45936</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>6</v>
@@ -2627,7 +2621,7 @@
         <v>1</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>10</v>
@@ -2635,13 +2629,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" s="1">
         <v>45936</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>5</v>
@@ -2656,7 +2650,7 @@
         <v>1</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>10</v>
@@ -2664,13 +2658,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" s="1">
         <v>45936</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>2</v>
@@ -2685,7 +2679,7 @@
         <v>1</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>10</v>
@@ -2693,14 +2687,14 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B57" s="1">
         <f>Tabela134[[#This Row],[SUBSTITUICAO DO ORING]]</f>
         <v>45957</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>8</v>
@@ -2715,7 +2709,7 @@
         <v>1</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>10</v>
@@ -2723,13 +2717,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B58" s="1">
         <v>45642</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>7</v>
@@ -2744,7 +2738,7 @@
         <v>1</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>0</v>
@@ -2752,13 +2746,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B59" s="1">
         <v>45853</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>6</v>
@@ -2773,7 +2767,7 @@
         <v>1</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>0</v>
@@ -2781,13 +2775,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B60" s="1">
         <v>45723</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>5</v>
@@ -2802,7 +2796,7 @@
         <v>1</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>0</v>
@@ -2810,13 +2804,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B61" s="1">
         <v>45853</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>2</v>
@@ -2831,7 +2825,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>0</v>
@@ -2839,13 +2833,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B62" s="1">
         <v>45818</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>8</v>
@@ -2860,7 +2854,7 @@
         <v>1</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>0</v>
@@ -2868,13 +2862,13 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B63" s="1">
         <v>45776</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>7</v>
@@ -2889,7 +2883,7 @@
         <v>1</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>0</v>
@@ -2897,13 +2891,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B64" s="1">
         <v>45818</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
@@ -2918,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>0</v>
@@ -2926,13 +2920,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B65" s="1">
         <v>45776</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>5</v>
@@ -2947,7 +2941,7 @@
         <v>1</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>0</v>
@@ -2955,13 +2949,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B66" s="1">
         <v>45894</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>2</v>
@@ -2976,7 +2970,7 @@
         <v>1</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>0</v>
@@ -2984,13 +2978,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B67" s="1">
         <v>45898</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>8</v>
@@ -3005,7 +2999,7 @@
         <v>1</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>0</v>
@@ -3013,13 +3007,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B68" s="1">
         <v>45898</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>7</v>
@@ -3034,7 +3028,7 @@
         <v>1</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>0</v>
@@ -3042,13 +3036,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B69" s="1">
         <v>45897</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>6</v>
@@ -3063,7 +3057,7 @@
         <v>1</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>0</v>
@@ -3071,13 +3065,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B70" s="1">
         <v>45897</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>5</v>
@@ -3092,7 +3086,7 @@
         <v>1</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>0</v>
@@ -3100,13 +3094,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B71" s="1">
         <v>45897</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>2</v>
@@ -3121,7 +3115,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>0</v>
@@ -3129,13 +3123,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B72" s="1">
         <v>45616</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>8</v>
@@ -3150,7 +3144,7 @@
         <v>1</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>0</v>
@@ -3158,13 +3152,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B73" s="1">
         <v>45624</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>7</v>
@@ -3179,7 +3173,7 @@
         <v>1</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>0</v>
@@ -3187,13 +3181,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B74" s="1">
         <v>45616</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>6</v>
@@ -3208,7 +3202,7 @@
         <v>1</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>0</v>
@@ -3216,13 +3210,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B75" s="1">
         <v>45846</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>5</v>
@@ -3237,7 +3231,7 @@
         <v>1</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>0</v>
@@ -3245,13 +3239,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B76" s="1">
         <v>45846</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>2</v>
@@ -3266,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>0</v>
@@ -3274,13 +3268,13 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B77" s="1">
         <v>45895</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>8</v>
@@ -3295,7 +3289,7 @@
         <v>1</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>0</v>
@@ -3303,13 +3297,13 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B78" s="1">
         <v>45895</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>7</v>
@@ -3324,7 +3318,7 @@
         <v>1</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>0</v>
@@ -3332,14 +3326,14 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B79" s="1">
         <f>Tabela134[[#This Row],[SUBSTITUICAO DO ORING]]</f>
         <v>45905</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>6</v>
@@ -3354,7 +3348,7 @@
         <v>1</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>0</v>
@@ -3362,13 +3356,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B80" s="1">
         <v>45973</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>5</v>
@@ -3383,7 +3377,7 @@
         <v>1</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>10</v>
@@ -3391,14 +3385,14 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B81" s="1">
         <f>Tabela134[[#This Row],[SUBSTITUICAO DO ORING]]</f>
         <v>45905</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>2</v>
@@ -3413,7 +3407,7 @@
         <v>1</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>0</v>
@@ -3421,13 +3415,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B82" s="1">
         <v>45916</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>8</v>
@@ -3442,7 +3436,7 @@
         <v>1</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>10</v>
@@ -3450,13 +3444,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B83" s="1">
         <v>45915</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>7</v>
@@ -3471,7 +3465,7 @@
         <v>1</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>10</v>
@@ -3479,13 +3473,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B84" s="1">
         <v>45916</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>6</v>
@@ -3500,7 +3494,7 @@
         <v>1</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>10</v>
@@ -3508,13 +3502,13 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B85" s="1">
         <v>45915</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>5</v>
@@ -3529,7 +3523,7 @@
         <v>1</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>10</v>
@@ -3537,13 +3531,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B86" s="1">
         <v>45916</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>2</v>
@@ -3558,7 +3552,7 @@
         <v>1</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>10</v>
@@ -3566,13 +3560,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B87" s="1">
         <v>45558</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>8</v>
@@ -3587,7 +3581,7 @@
         <v>1</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>0</v>
@@ -3595,13 +3589,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B88" s="1">
         <v>45565</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>7</v>
@@ -3616,7 +3610,7 @@
         <v>1</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>0</v>
@@ -3624,13 +3618,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B89" s="1">
         <v>45643</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>6</v>
@@ -3645,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>0</v>
@@ -3653,13 +3647,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B90" s="1">
         <v>45702</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>5</v>
@@ -3674,7 +3668,7 @@
         <v>1</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>0</v>
@@ -3682,13 +3676,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B91" s="1">
         <v>45702</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>2</v>
@@ -3703,7 +3697,7 @@
         <v>1</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>0</v>
@@ -3711,13 +3705,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B92" s="1">
         <v>45845</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>8</v>
@@ -3732,7 +3726,7 @@
         <v>1</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>0</v>
@@ -3740,13 +3734,13 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B93" s="1">
         <v>45869</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>7</v>
@@ -3761,7 +3755,7 @@
         <v>1</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>0</v>
@@ -3769,13 +3763,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B94" s="1">
         <v>45869</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>6</v>
@@ -3790,7 +3784,7 @@
         <v>1</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>0</v>
@@ -3798,13 +3792,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B95" s="1">
         <v>45845</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>5</v>
@@ -3819,7 +3813,7 @@
         <v>1</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>0</v>
@@ -3827,13 +3821,13 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B96" s="1">
         <v>45869</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>2</v>
@@ -3848,7 +3842,7 @@
         <v>1</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>0</v>
@@ -3856,13 +3850,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B97" s="1">
         <v>45884</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>8</v>
@@ -3877,7 +3871,7 @@
         <v>1</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>0</v>
@@ -3885,13 +3879,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B98" s="1">
         <v>45883</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>7</v>
@@ -3906,7 +3900,7 @@
         <v>1</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>0</v>
@@ -3914,13 +3908,13 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B99" s="1">
         <v>45884</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>6</v>
@@ -3935,7 +3929,7 @@
         <v>1</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>0</v>
@@ -3943,13 +3937,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B100" s="1">
         <v>45883</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>5</v>
@@ -3964,7 +3958,7 @@
         <v>1</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>0</v>
@@ -3972,13 +3966,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B101" s="1">
         <v>45883</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>2</v>
@@ -3993,7 +3987,7 @@
         <v>1</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>0</v>
@@ -4001,13 +3995,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B102" s="1">
         <v>45911</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>8</v>
@@ -4022,7 +4016,7 @@
         <v>1</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>10</v>
@@ -4030,13 +4024,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B103" s="1">
         <v>45866</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>7</v>
@@ -4051,7 +4045,7 @@
         <v>1</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>10</v>
@@ -4059,13 +4053,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B104" s="1">
         <v>45866</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>6</v>
@@ -4080,7 +4074,7 @@
         <v>1</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>10</v>
@@ -4088,13 +4082,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B105" s="1">
         <v>45911</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>5</v>
@@ -4109,7 +4103,7 @@
         <v>1</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>10</v>
@@ -4117,13 +4111,13 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B106" s="1">
         <v>45911</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>2</v>
@@ -4138,7 +4132,7 @@
         <v>1</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>10</v>
@@ -4146,13 +4140,13 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B107" s="1">
         <v>45835</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>8</v>
@@ -4167,7 +4161,7 @@
         <v>1</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>0</v>
@@ -4175,13 +4169,13 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B108" s="1">
         <v>45645</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>7</v>
@@ -4196,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>0</v>
@@ -4204,13 +4198,13 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B109" s="1">
         <v>45835</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>6</v>
@@ -4225,7 +4219,7 @@
         <v>1</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>0</v>
@@ -4233,13 +4227,13 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B110" s="1">
         <v>45861</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>5</v>
@@ -4254,7 +4248,7 @@
         <v>1</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>0</v>
@@ -4262,13 +4256,13 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B111" s="1">
         <v>45861</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>2</v>
@@ -4283,7 +4277,7 @@
         <v>1</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>0</v>
@@ -4291,13 +4285,13 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B112" s="1">
         <v>45827</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>8</v>
@@ -4312,21 +4306,21 @@
         <v>1</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B113" s="1">
         <v>45652</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>7</v>
@@ -4341,21 +4335,21 @@
         <v>1</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B114" s="1">
         <v>45827</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>6</v>
@@ -4370,7 +4364,7 @@
         <v>1</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>10</v>
@@ -4378,13 +4372,13 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B115" s="1">
         <v>45903</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>5</v>
@@ -4399,7 +4393,7 @@
         <v>1</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>10</v>
@@ -4407,13 +4401,13 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B116" s="1">
         <v>45903</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>2</v>
@@ -4428,7 +4422,7 @@
         <v>1</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>10</v>
@@ -4436,13 +4430,13 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B117" s="1">
         <v>45918</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>8</v>
@@ -4457,7 +4451,7 @@
         <v>1</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>10</v>
@@ -4465,13 +4459,13 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B118" s="1">
         <v>45917</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>7</v>
@@ -4486,7 +4480,7 @@
         <v>1</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>10</v>
@@ -4494,13 +4488,13 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B119" s="1">
         <v>45918</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>6</v>
@@ -4515,7 +4509,7 @@
         <v>1</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I119" s="2" t="s">
         <v>10</v>
@@ -4523,13 +4517,13 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B120" s="1">
         <v>45917</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>5</v>
@@ -4544,7 +4538,7 @@
         <v>1</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>10</v>
@@ -4552,13 +4546,13 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B121" s="1">
         <v>45918</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>2</v>
@@ -4573,7 +4567,7 @@
         <v>1</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I121" s="2" t="s">
         <v>10</v>
@@ -4581,13 +4575,13 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B122" s="1">
         <v>45817</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>8</v>
@@ -4602,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>0</v>
@@ -4610,13 +4604,13 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B123" s="1">
         <v>45817</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>7</v>
@@ -4631,7 +4625,7 @@
         <v>1</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>0</v>
@@ -4639,13 +4633,13 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B124" s="1">
         <v>45887</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>6</v>
@@ -4660,7 +4654,7 @@
         <v>1</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>0</v>
@@ -4668,13 +4662,13 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B125" s="1">
         <v>45887</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>5</v>
@@ -4689,7 +4683,7 @@
         <v>1</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I125" s="1" t="s">
         <v>0</v>
@@ -4697,13 +4691,13 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B126" s="1">
         <v>45887</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>2</v>
@@ -4718,7 +4712,7 @@
         <v>1</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I126" s="1" t="s">
         <v>0</v>
@@ -4726,13 +4720,13 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B127" s="1">
         <v>45909</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>8</v>
@@ -4747,7 +4741,7 @@
         <v>1</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I127" s="2" t="s">
         <v>10</v>
@@ -4755,13 +4749,13 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B128" s="1">
         <v>45909</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>7</v>
@@ -4776,7 +4770,7 @@
         <v>1</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I128" s="2" t="s">
         <v>10</v>
@@ -4784,13 +4778,13 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B129" s="1">
         <v>45910</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>6</v>
@@ -4805,7 +4799,7 @@
         <v>1</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I129" s="2" t="s">
         <v>10</v>
@@ -4813,13 +4807,13 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B130" s="1">
         <v>45910</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>5</v>
@@ -4834,7 +4828,7 @@
         <v>1</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I130" s="2" t="s">
         <v>10</v>
@@ -4842,13 +4836,13 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B131" s="1">
         <v>45910</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>2</v>
@@ -4863,7 +4857,7 @@
         <v>1</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I131" s="2" t="s">
         <v>10</v>
@@ -4871,13 +4865,13 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B132" s="1">
         <v>45896</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>8</v>
@@ -4892,7 +4886,7 @@
         <v>1</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>0</v>
@@ -4900,13 +4894,13 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B133" s="1">
         <v>45790</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>7</v>
@@ -4921,7 +4915,7 @@
         <v>1</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I133" s="1" t="s">
         <v>0</v>
@@ -4929,13 +4923,13 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B134" s="1">
         <v>45834</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>6</v>
@@ -4950,7 +4944,7 @@
         <v>1</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I134" s="1" t="s">
         <v>0</v>
@@ -4958,13 +4952,13 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B135" s="1">
         <v>45834</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>5</v>
@@ -4979,7 +4973,7 @@
         <v>1</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I135" s="1" t="s">
         <v>0</v>
@@ -4987,13 +4981,13 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B136" s="1">
         <v>45896</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>2</v>
@@ -5008,7 +5002,7 @@
         <v>1</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I136" s="1" t="s">
         <v>0</v>
@@ -5016,13 +5010,13 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B137" s="1">
         <v>45705</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>8</v>
@@ -5037,7 +5031,7 @@
         <v>1</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I137" s="1" t="s">
         <v>0</v>
@@ -5045,13 +5039,13 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B138" s="1">
         <v>45560</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>7</v>
@@ -5066,7 +5060,7 @@
         <v>1</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I138" s="1" t="s">
         <v>0</v>
@@ -5074,13 +5068,13 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B139" s="1">
         <v>45705</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>6</v>
@@ -5095,7 +5089,7 @@
         <v>1</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I139" s="1" t="s">
         <v>0</v>
@@ -5103,13 +5097,13 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B140" s="1">
         <v>45785</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>5</v>
@@ -5124,7 +5118,7 @@
         <v>1</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I140" s="1" t="s">
         <v>0</v>
@@ -5132,13 +5126,13 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B141" s="1">
         <v>45785</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>2</v>
@@ -5153,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I141" s="1" t="s">
         <v>0</v>
@@ -5161,13 +5155,13 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B142" s="1">
         <v>45852</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>8</v>
@@ -5182,7 +5176,7 @@
         <v>1</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I142" s="1" t="s">
         <v>0</v>
@@ -5190,13 +5184,13 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B143" s="1">
         <v>45646</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>7</v>
@@ -5211,7 +5205,7 @@
         <v>1</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I143" s="1" t="s">
         <v>0</v>
@@ -5219,13 +5213,13 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B144" s="1">
         <v>45852</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>6</v>
@@ -5240,7 +5234,7 @@
         <v>1</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>0</v>
@@ -5248,13 +5242,13 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B145" s="1">
         <v>45904</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>5</v>
@@ -5269,7 +5263,7 @@
         <v>1</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I145" s="1" t="s">
         <v>10</v>
@@ -5277,13 +5271,13 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B146" s="1">
         <v>45772</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>2</v>
@@ -5298,7 +5292,7 @@
         <v>1</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I146" s="1" t="s">
         <v>10</v>
@@ -5306,13 +5300,13 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B147" s="1">
         <v>45555</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>8</v>
@@ -5327,7 +5321,7 @@
         <v>1</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I147" s="1" t="s">
         <v>0</v>
@@ -5335,13 +5329,13 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B148" s="1">
         <v>45647</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>7</v>
@@ -5356,7 +5350,7 @@
         <v>1</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>0</v>
@@ -5364,13 +5358,13 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B149" s="1">
         <v>45647</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>6</v>
@@ -5385,7 +5379,7 @@
         <v>1</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>0</v>
@@ -5393,13 +5387,13 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B150" s="1">
         <v>45342</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>5</v>
@@ -5414,7 +5408,7 @@
         <v>1</v>
       </c>
       <c r="H150" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>0</v>
@@ -5422,13 +5416,13 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B151" s="1">
         <v>45342</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>2</v>
@@ -5443,7 +5437,7 @@
         <v>1</v>
       </c>
       <c r="H151" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>0</v>
@@ -5451,13 +5445,13 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B152" s="1">
         <v>45953</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>8</v>
@@ -5472,7 +5466,7 @@
         <v>1</v>
       </c>
       <c r="H152" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I152" s="1" t="s">
         <v>10</v>
@@ -5480,13 +5474,13 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B153" s="1">
         <v>45953</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>7</v>
@@ -5501,7 +5495,7 @@
         <v>1</v>
       </c>
       <c r="H153" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I153" s="1" t="s">
         <v>10</v>
@@ -5509,13 +5503,13 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B154" s="1">
         <v>45727</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>6</v>
@@ -5530,7 +5524,7 @@
         <v>1</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I154" s="1" t="s">
         <v>10</v>
@@ -5538,13 +5532,13 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B155" s="1">
         <v>45860</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>5</v>
@@ -5559,7 +5553,7 @@
         <v>1</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I155" s="1" t="s">
         <v>10</v>
@@ -5567,13 +5561,13 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B156" s="1">
         <v>45860</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>2</v>
@@ -5588,7 +5582,7 @@
         <v>1</v>
       </c>
       <c r="H156" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I156" s="1" t="s">
         <v>10</v>
@@ -5596,13 +5590,13 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B157" s="1">
         <v>45908</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>8</v>
@@ -5617,7 +5611,7 @@
         <v>1</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I157" s="2" t="s">
         <v>10</v>
@@ -5625,13 +5619,13 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B158" s="1">
         <v>45503</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>7</v>
@@ -5646,7 +5640,7 @@
         <v>1</v>
       </c>
       <c r="H158" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I158" s="2" t="s">
         <v>10</v>
@@ -5654,13 +5648,13 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B159" s="1">
         <v>45825</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>6</v>
@@ -5675,21 +5669,21 @@
         <v>1</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B160" s="1">
         <v>45825</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>5</v>
@@ -5704,7 +5698,7 @@
         <v>1</v>
       </c>
       <c r="H160" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I160" s="2" t="s">
         <v>10</v>
@@ -5712,13 +5706,13 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B161" s="1">
         <v>45908</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>2</v>
@@ -5733,7 +5727,7 @@
         <v>1</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I161" s="2" t="s">
         <v>10</v>
@@ -5741,13 +5735,13 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B162" s="1">
         <v>45666</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>8</v>
@@ -5762,7 +5756,7 @@
         <v>1</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I162" s="1" t="s">
         <v>0</v>
@@ -5770,13 +5764,13 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B163" s="1">
         <v>45666</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>7</v>
@@ -5791,7 +5785,7 @@
         <v>1</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I163" s="1" t="s">
         <v>0</v>
@@ -5799,13 +5793,13 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B164" s="1">
         <v>45826</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>6</v>
@@ -5820,7 +5814,7 @@
         <v>1</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I164" s="1" t="s">
         <v>0</v>
@@ -5828,13 +5822,13 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B165" s="1">
         <v>45826</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>5</v>
@@ -5849,7 +5843,7 @@
         <v>1</v>
       </c>
       <c r="H165" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I165" s="1" t="s">
         <v>0</v>
@@ -5857,13 +5851,13 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B166" s="1">
         <v>45926</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>2</v>
@@ -5878,7 +5872,7 @@
         <v>1</v>
       </c>
       <c r="H166" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I166" s="1" t="s">
         <v>10</v>
@@ -5892,7 +5886,7 @@
         <v>45806</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>8</v>
@@ -5907,7 +5901,7 @@
         <v>1</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I167" s="1" t="s">
         <v>10</v>
@@ -5921,7 +5915,7 @@
         <v>45891</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>7</v>
@@ -5936,7 +5930,7 @@
         <v>1</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I168" s="1" t="s">
         <v>10</v>
@@ -5950,7 +5944,7 @@
         <v>45806</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>6</v>
@@ -5965,7 +5959,7 @@
         <v>1</v>
       </c>
       <c r="H169" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I169" s="1" t="s">
         <v>10</v>
@@ -5979,7 +5973,7 @@
         <v>45891</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>5</v>
@@ -5994,7 +5988,7 @@
         <v>1</v>
       </c>
       <c r="H170" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I170" s="1" t="s">
         <v>10</v>
@@ -6008,7 +6002,7 @@
         <v>45891</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>2</v>
@@ -6023,7 +6017,7 @@
         <v>1</v>
       </c>
       <c r="H171" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I171" s="1" t="s">
         <v>10</v>
@@ -6052,7 +6046,7 @@
         <v>1</v>
       </c>
       <c r="H172" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I172" s="1" t="s">
         <v>0</v>
@@ -6081,7 +6075,7 @@
         <v>1</v>
       </c>
       <c r="H173" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I173" s="1" t="s">
         <v>0</v>
@@ -6110,7 +6104,7 @@
         <v>1</v>
       </c>
       <c r="H174" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I174" s="1" t="s">
         <v>0</v>
@@ -6139,7 +6133,7 @@
         <v>1</v>
       </c>
       <c r="H175" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I175" s="1" t="s">
         <v>0</v>
@@ -6168,7 +6162,7 @@
         <v>1</v>
       </c>
       <c r="H176" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I176" s="1" t="s">
         <v>0</v>
@@ -6197,7 +6191,7 @@
         <v>1</v>
       </c>
       <c r="H177" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I177" s="1" t="s">
         <v>0</v>
@@ -6226,7 +6220,7 @@
         <v>1</v>
       </c>
       <c r="H178" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I178" s="1" t="s">
         <v>0</v>
@@ -6255,7 +6249,7 @@
         <v>1</v>
       </c>
       <c r="H179" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I179" s="1" t="s">
         <v>0</v>
@@ -6284,7 +6278,7 @@
         <v>1</v>
       </c>
       <c r="H180" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I180" s="2" t="s">
         <v>10</v>
@@ -6313,7 +6307,7 @@
         <v>1</v>
       </c>
       <c r="H181" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I181" s="2" t="s">
         <v>10</v>
@@ -6342,7 +6336,7 @@
         <v>1</v>
       </c>
       <c r="H182" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I182" s="2" t="s">
         <v>28</v>
@@ -6371,7 +6365,7 @@
         <v>1</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I183" s="2" t="s">
         <v>16</v>
@@ -6400,7 +6394,7 @@
         <v>1</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I184" s="2" t="s">
         <v>27</v>
@@ -6429,7 +6423,7 @@
         <v>1</v>
       </c>
       <c r="H185" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I185" s="2" t="s">
         <v>26</v>
@@ -6458,7 +6452,7 @@
         <v>1</v>
       </c>
       <c r="H186" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I186" s="2" t="s">
         <v>24</v>
@@ -6487,7 +6481,7 @@
         <v>1</v>
       </c>
       <c r="H187" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I187" s="1" t="s">
         <v>0</v>
@@ -6516,7 +6510,7 @@
         <v>1</v>
       </c>
       <c r="H188" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I188" s="1" t="s">
         <v>0</v>
@@ -6545,7 +6539,7 @@
         <v>1</v>
       </c>
       <c r="H189" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I189" s="1" t="s">
         <v>0</v>
@@ -6574,7 +6568,7 @@
         <v>1</v>
       </c>
       <c r="H190" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I190" s="1" t="s">
         <v>0</v>
@@ -6603,7 +6597,7 @@
         <v>1</v>
       </c>
       <c r="H191" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I191" s="1" t="s">
         <v>0</v>
@@ -6632,7 +6626,7 @@
         <v>1</v>
       </c>
       <c r="H192" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I192" s="1" t="s">
         <v>0</v>
@@ -6661,7 +6655,7 @@
         <v>1</v>
       </c>
       <c r="H193" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I193" s="1" t="s">
         <v>0</v>
@@ -6690,7 +6684,7 @@
         <v>1</v>
       </c>
       <c r="H194" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I194" s="1" t="s">
         <v>0</v>
@@ -6719,7 +6713,7 @@
         <v>1</v>
       </c>
       <c r="H195" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I195" s="2" t="s">
         <v>10</v>
@@ -6748,7 +6742,7 @@
         <v>1</v>
       </c>
       <c r="H196" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I196" s="1" t="s">
         <v>0</v>
@@ -6777,7 +6771,7 @@
         <v>1</v>
       </c>
       <c r="H197" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I197" s="1" t="s">
         <v>0</v>
@@ -6806,7 +6800,7 @@
         <v>1</v>
       </c>
       <c r="H198" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I198" s="1" t="s">
         <v>0</v>
@@ -6835,7 +6829,7 @@
         <v>1</v>
       </c>
       <c r="H199" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I199" s="1" t="s">
         <v>0</v>
@@ -6864,7 +6858,7 @@
         <v>1</v>
       </c>
       <c r="H200" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I200" s="1" t="s">
         <v>0</v>
@@ -6893,7 +6887,7 @@
         <v>1</v>
       </c>
       <c r="H201" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I201" s="1" t="s">
         <v>0</v>
@@ -6922,7 +6916,7 @@
         <v>1</v>
       </c>
       <c r="H202" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I202" s="1" t="s">
         <v>10</v>
@@ -6951,7 +6945,7 @@
         <v>1</v>
       </c>
       <c r="H203" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I203" s="1" t="s">
         <v>0</v>
@@ -6980,7 +6974,7 @@
         <v>1</v>
       </c>
       <c r="H204" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I204" s="1" t="s">
         <v>10</v>
@@ -7009,7 +7003,7 @@
         <v>1</v>
       </c>
       <c r="H205" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I205" s="1" t="s">
         <v>10</v>
@@ -7038,7 +7032,7 @@
         <v>1</v>
       </c>
       <c r="H206" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I206" s="1" t="s">
         <v>10</v>
@@ -7067,7 +7061,7 @@
         <v>1</v>
       </c>
       <c r="H207" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I207" s="2" t="s">
         <v>19</v>
@@ -7096,7 +7090,7 @@
         <v>1</v>
       </c>
       <c r="H208" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I208" s="2" t="s">
         <v>18</v>
@@ -7125,7 +7119,7 @@
         <v>1</v>
       </c>
       <c r="H209" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I209" s="2" t="s">
         <v>17</v>
@@ -7154,7 +7148,7 @@
         <v>1</v>
       </c>
       <c r="H210" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I210" s="2" t="s">
         <v>16</v>
@@ -7183,7 +7177,7 @@
         <v>1</v>
       </c>
       <c r="H211" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I211" s="2" t="s">
         <v>14</v>
@@ -7212,7 +7206,7 @@
         <v>1</v>
       </c>
       <c r="H212" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I212" s="1" t="s">
         <v>0</v>
@@ -7241,7 +7235,7 @@
         <v>1</v>
       </c>
       <c r="H213" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I213" s="1" t="s">
         <v>0</v>
@@ -7270,7 +7264,7 @@
         <v>1</v>
       </c>
       <c r="H214" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I214" s="1" t="s">
         <v>0</v>
@@ -7299,7 +7293,7 @@
         <v>1</v>
       </c>
       <c r="H215" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I215" s="1" t="s">
         <v>0</v>
@@ -7328,7 +7322,7 @@
         <v>1</v>
       </c>
       <c r="H216" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I216" s="1" t="s">
         <v>0</v>
@@ -7357,7 +7351,7 @@
         <v>1</v>
       </c>
       <c r="H217" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I217" s="1" t="s">
         <v>0</v>
@@ -7386,7 +7380,7 @@
         <v>1</v>
       </c>
       <c r="H218" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I218" s="1" t="s">
         <v>0</v>
@@ -7415,7 +7409,7 @@
         <v>1</v>
       </c>
       <c r="H219" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I219" s="1" t="s">
         <v>0</v>
@@ -7444,7 +7438,7 @@
         <v>1</v>
       </c>
       <c r="H220" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I220" s="1" t="s">
         <v>0</v>
@@ -7473,7 +7467,7 @@
         <v>1</v>
       </c>
       <c r="H221" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I221" s="1" t="s">
         <v>0</v>
@@ -7502,7 +7496,7 @@
         <v>1</v>
       </c>
       <c r="H222" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I222" s="1" t="s">
         <v>0</v>
@@ -7531,7 +7525,7 @@
         <v>1</v>
       </c>
       <c r="H223" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I223" s="1" t="s">
         <v>0</v>
@@ -7560,7 +7554,7 @@
         <v>1</v>
       </c>
       <c r="H224" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I224" s="1" t="s">
         <v>0</v>
@@ -7589,7 +7583,7 @@
         <v>1</v>
       </c>
       <c r="H225" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I225" s="1" t="s">
         <v>0</v>
@@ -7618,7 +7612,7 @@
         <v>1</v>
       </c>
       <c r="H226" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I226" s="1" t="s">
         <v>0</v>
@@ -7647,7 +7641,7 @@
         <v>1</v>
       </c>
       <c r="H227" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I227" s="1" t="s">
         <v>0</v>
@@ -7676,7 +7670,7 @@
         <v>1</v>
       </c>
       <c r="H228" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I228" s="1" t="s">
         <v>0</v>
@@ -7705,7 +7699,7 @@
         <v>1</v>
       </c>
       <c r="H229" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I229" s="2" t="s">
         <v>10</v>
@@ -7734,7 +7728,7 @@
         <v>1</v>
       </c>
       <c r="H230" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I230" s="1" t="s">
         <v>0</v>
@@ -7763,7 +7757,7 @@
         <v>1</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I231" s="1" t="s">
         <v>0</v>
@@ -7792,7 +7786,7 @@
         <v>1</v>
       </c>
       <c r="H232" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I232" s="1" t="s">
         <v>0</v>
@@ -7821,7 +7815,7 @@
         <v>1</v>
       </c>
       <c r="H233" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I233" s="1" t="s">
         <v>0</v>
@@ -7850,7 +7844,7 @@
         <v>1</v>
       </c>
       <c r="H234" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I234" s="1" t="s">
         <v>0</v>
@@ -7879,7 +7873,7 @@
         <v>1</v>
       </c>
       <c r="H235" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I235" s="1" t="s">
         <v>0</v>
@@ -7908,19 +7902,14 @@
         <v>1</v>
       </c>
       <c r="H236" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I236" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E242" s="14">
-        <v>45905</v>
-      </c>
-      <c r="F242" t="s">
-        <v>86</v>
-      </c>
+    <row r="242" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E242" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H236">
@@ -7965,11 +7954,11 @@
   <sheetData>
     <row r="3" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D3" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="15"/>
       <c r="G3" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H3" s="15"/>
     </row>

</xml_diff>